<commit_message>
Gulf Edge details updated
</commit_message>
<xml_diff>
--- a/ASRProps-Final.xlsx
+++ b/ASRProps-Final.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24026"/>
+  <workbookPr defaultThemeVersion="166925"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/a063b81c7d42b926/Documents/ASR-Props/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="8" documentId="11_B65B585BC469815E41FBBAE2ED8C4BDFAD7A2CD5" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{71E0437A-9D52-4D41-A90A-0F30A2340369}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="5" r:id="rId1"/>
@@ -12,14 +18,14 @@
     <sheet name="Home" sheetId="4" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Property Details'!$A$1:$Q$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Property Details'!$A$1:$R$45</definedName>
   </definedNames>
   <calcPr calcId="124519"/>
   <pivotCaches>
-    <pivotCache cacheId="13" r:id="rId4"/>
+    <pivotCache cacheId="0" r:id="rId4"/>
   </pivotCaches>
-  <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+  <extLst>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -27,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="582" uniqueCount="272">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="641" uniqueCount="292">
   <si>
     <t>S No</t>
   </si>
@@ -850,13 +856,73 @@
   </si>
   <si>
     <t>https://www.google.com/maps/place/17%C2%B026'03.5%22N+78%C2%B023'54.9%22E/@17.434108,78.3987006,20z/data=!4m5!3m4!1s0x0:0x0!8m2!3d17.4343089!4d78.3985933?hl=en</t>
+  </si>
+  <si>
+    <t>Dimension B/W</t>
+  </si>
+  <si>
+    <t>1000 to 1200</t>
+  </si>
+  <si>
+    <t>1200 to 1500</t>
+  </si>
+  <si>
+    <t>100 +Acers</t>
+  </si>
+  <si>
+    <t>1500 to 2000</t>
+  </si>
+  <si>
+    <t>100 to 500</t>
+  </si>
+  <si>
+    <t>1 to 5 Acers</t>
+  </si>
+  <si>
+    <t>2000 to 2500</t>
+  </si>
+  <si>
+    <t>2500 to 3000</t>
+  </si>
+  <si>
+    <t>3000 to 4000</t>
+  </si>
+  <si>
+    <t>5 to 10 Acers</t>
+  </si>
+  <si>
+    <t>500 to 1000</t>
+  </si>
+  <si>
+    <t>More than 5000</t>
+  </si>
+  <si>
+    <t>Sudheer GMR</t>
+  </si>
+  <si>
+    <t>Plot No B 36</t>
+  </si>
+  <si>
+    <t>1400 sq Yards</t>
+  </si>
+  <si>
+    <t>Gulf Edge Residency</t>
+  </si>
+  <si>
+    <t>https://www.google.com/maps/place/Golf+Edge+Residence/@17.4245293,78.3453949,17z/data=!4m5!3m4!1s0x3bcb913572d58f8b:0xa6b7828ea4641aa2!8m2!3d17.4244285!4d78.3475787?hl=en</t>
+  </si>
+  <si>
+    <t>Nanakramguda</t>
+  </si>
+  <si>
+    <t>left from Wipro Circle</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="3">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -921,7 +987,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -956,11 +1022,14 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="29">
+  <dxfs count="18">
     <dxf>
       <border>
         <left style="thin">
@@ -1009,153 +1078,6 @@
           <color indexed="64"/>
         </left>
       </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" readingOrder="0"/>
     </dxf>
     <dxf>
       <alignment horizontal="center" readingOrder="0"/>
@@ -1318,9 +1240,9 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1" refreshedBy="Aryan" refreshedDate="44373.452933101849" createdVersion="3" refreshedVersion="3" minRefreshableVersion="3" recordCount="44">
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="Aryan" refreshedDate="44373.452933101849" createdVersion="3" refreshedVersion="3" minRefreshableVersion="3" recordCount="44" xr:uid="{00000000-000A-0000-FFFF-FFFF00000000}">
   <cacheSource type="worksheet">
-    <worksheetSource ref="A1:Q45" sheet="Property Details"/>
+    <worksheetSource ref="A1:R45" sheet="Property Details"/>
   </cacheSource>
   <cacheFields count="17">
     <cacheField name="S No" numFmtId="0">
@@ -1449,6 +1371,11 @@
       <sharedItems containsBlank="1" longText="1"/>
     </cacheField>
   </cacheFields>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{725AE2AE-9491-48be-B2B4-4EB974FC3084}">
+      <x14:pivotCacheDefinition/>
+    </ext>
+  </extLst>
 </pivotCacheDefinition>
 </file>
 
@@ -2294,7 +2221,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable1" cacheId="13" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="3" minRefreshableVersion="3" showCalcMbrs="0" useAutoFormatting="1" itemPrintTitles="1" createdVersion="3" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0000-000000000000}" name="PivotTable1" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="3" minRefreshableVersion="3" showCalcMbrs="0" useAutoFormatting="1" itemPrintTitles="1" createdVersion="3" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A3:E72" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="17">
     <pivotField showAll="0"/>
@@ -2632,49 +2559,49 @@
     <dataField name="Count of Sale / Devlop" fld="8" subtotal="count" baseField="0" baseItem="0"/>
   </dataFields>
   <formats count="18">
-    <format dxfId="28">
+    <format dxfId="17">
       <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
     </format>
-    <format dxfId="27">
+    <format dxfId="16">
       <pivotArea field="1" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="0"/>
     </format>
-    <format dxfId="26">
+    <format dxfId="15">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="1" count="0"/>
         </references>
       </pivotArea>
     </format>
-    <format dxfId="25">
+    <format dxfId="14">
       <pivotArea dataOnly="0" labelOnly="1" grandRow="1" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="24">
+    <format dxfId="13">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="8" count="0"/>
         </references>
       </pivotArea>
     </format>
-    <format dxfId="23">
+    <format dxfId="12">
       <pivotArea dataOnly="0" labelOnly="1" grandCol="1" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="22">
+    <format dxfId="11">
       <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
     </format>
-    <format dxfId="21">
+    <format dxfId="10">
       <pivotArea field="8" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisCol" fieldPosition="0"/>
     </format>
-    <format dxfId="20">
+    <format dxfId="9">
       <pivotArea type="topRight" dataOnly="0" labelOnly="1" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="19">
+    <format dxfId="8">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="8" count="0"/>
         </references>
       </pivotArea>
     </format>
-    <format dxfId="18">
+    <format dxfId="7">
       <pivotArea dataOnly="0" labelOnly="1" grandCol="1" outline="0" fieldPosition="0"/>
     </format>
     <format dxfId="6">
@@ -2715,6 +2642,11 @@
     </format>
   </formats>
   <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
+  </extLst>
 </pivotTableDefinition>
 </file>
 
@@ -3007,21 +2939,21 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A3:E72"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="24.109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="17.77734375" style="12" bestFit="1" customWidth="1"/>
@@ -3036,7 +2968,7 @@
     <col min="11" max="11" width="10.77734375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="8" t="s">
         <v>213</v>
       </c>
@@ -3044,7 +2976,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="9" t="s">
         <v>210</v>
       </c>
@@ -3061,7 +2993,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="5" spans="1:5">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="10" t="s">
         <v>25</v>
       </c>
@@ -3074,7 +3006,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:5">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" s="11" t="s">
         <v>264</v>
       </c>
@@ -3087,7 +3019,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:5">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" s="11" t="s">
         <v>252</v>
       </c>
@@ -3100,7 +3032,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:5">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" s="11" t="s">
         <v>261</v>
       </c>
@@ -3113,7 +3045,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:5">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" s="11" t="s">
         <v>80</v>
       </c>
@@ -3126,7 +3058,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:5">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" s="11" t="s">
         <v>190</v>
       </c>
@@ -3139,7 +3071,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:5">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" s="10" t="s">
         <v>242</v>
       </c>
@@ -3152,7 +3084,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:5">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" s="11" t="s">
         <v>195</v>
       </c>
@@ -3165,7 +3097,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:5">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" s="10" t="s">
         <v>172</v>
       </c>
@@ -3178,7 +3110,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="14" spans="1:5">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" s="11" t="s">
         <v>122</v>
       </c>
@@ -3191,7 +3123,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:5">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" s="11" t="s">
         <v>174</v>
       </c>
@@ -3204,7 +3136,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:5">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" s="10" t="s">
         <v>94</v>
       </c>
@@ -3217,7 +3149,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:5">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" s="11" t="s">
         <v>95</v>
       </c>
@@ -3230,7 +3162,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:5">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" s="10" t="s">
         <v>194</v>
       </c>
@@ -3243,7 +3175,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:5">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19" s="11" t="s">
         <v>195</v>
       </c>
@@ -3256,7 +3188,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:5">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20" s="10" t="s">
         <v>79</v>
       </c>
@@ -3269,7 +3201,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:5">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21" s="11" t="s">
         <v>80</v>
       </c>
@@ -3282,7 +3214,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:5">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22" s="10" t="s">
         <v>144</v>
       </c>
@@ -3295,7 +3227,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:5">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A23" s="11" t="s">
         <v>80</v>
       </c>
@@ -3308,7 +3240,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:5">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A24" s="10" t="s">
         <v>20</v>
       </c>
@@ -3321,7 +3253,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="25" spans="1:5">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A25" s="11" t="s">
         <v>134</v>
       </c>
@@ -3334,7 +3266,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:5">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A26" s="11" t="s">
         <v>15</v>
       </c>
@@ -3347,7 +3279,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:5">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A27" s="10" t="s">
         <v>152</v>
       </c>
@@ -3360,7 +3292,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:5">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A28" s="11" t="s">
         <v>153</v>
       </c>
@@ -3373,7 +3305,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:5">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A29" s="10" t="s">
         <v>101</v>
       </c>
@@ -3386,7 +3318,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:5">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A30" s="11" t="s">
         <v>102</v>
       </c>
@@ -3399,7 +3331,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:5">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A31" s="10" t="s">
         <v>115</v>
       </c>
@@ -3414,7 +3346,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="32" spans="1:5">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A32" s="11" t="s">
         <v>116</v>
       </c>
@@ -3427,7 +3359,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:5">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A33" s="11" t="s">
         <v>205</v>
       </c>
@@ -3440,7 +3372,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="1:5">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A34" s="10" t="s">
         <v>85</v>
       </c>
@@ -3453,7 +3385,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="1:5">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A35" s="11" t="s">
         <v>86</v>
       </c>
@@ -3466,7 +3398,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="1:5">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A36" s="10" t="s">
         <v>129</v>
       </c>
@@ -3479,7 +3411,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="1:5">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A37" s="11" t="s">
         <v>130</v>
       </c>
@@ -3492,7 +3424,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="1:5">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A38" s="10" t="s">
         <v>224</v>
       </c>
@@ -3505,7 +3437,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="1:5">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A39" s="11" t="s">
         <v>122</v>
       </c>
@@ -3518,7 +3450,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="40" spans="1:5">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A40" s="10" t="s">
         <v>231</v>
       </c>
@@ -3531,7 +3463,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="41" spans="1:5">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A41" s="11" t="s">
         <v>232</v>
       </c>
@@ -3544,7 +3476,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="42" spans="1:5">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A42" s="10" t="s">
         <v>164</v>
       </c>
@@ -3557,7 +3489,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="43" spans="1:5">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A43" s="11" t="s">
         <v>34</v>
       </c>
@@ -3570,7 +3502,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="44" spans="1:5">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A44" s="11" t="s">
         <v>165</v>
       </c>
@@ -3583,7 +3515,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="45" spans="1:5">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A45" s="10" t="s">
         <v>21</v>
       </c>
@@ -3596,7 +3528,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="46" spans="1:5">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A46" s="11" t="s">
         <v>10</v>
       </c>
@@ -3609,7 +3541,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="47" spans="1:5">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A47" s="10" t="s">
         <v>147</v>
       </c>
@@ -3622,7 +3554,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="48" spans="1:5">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A48" s="11" t="s">
         <v>270</v>
       </c>
@@ -3635,7 +3567,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="49" spans="1:5">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A49" s="11" t="s">
         <v>148</v>
       </c>
@@ -3648,7 +3580,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="50" spans="1:5">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A50" s="10" t="s">
         <v>139</v>
       </c>
@@ -3661,7 +3593,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="51" spans="1:5">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A51" s="11" t="s">
         <v>41</v>
       </c>
@@ -3674,7 +3606,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="52" spans="1:5">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A52" s="10" t="s">
         <v>246</v>
       </c>
@@ -3687,7 +3619,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="53" spans="1:5">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A53" s="11" t="s">
         <v>247</v>
       </c>
@@ -3700,7 +3632,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="54" spans="1:5">
+    <row r="54" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A54" s="10" t="s">
         <v>214</v>
       </c>
@@ -3713,7 +3645,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="55" spans="1:5">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A55" s="11" t="s">
         <v>215</v>
       </c>
@@ -3726,7 +3658,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="56" spans="1:5">
+    <row r="56" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A56" s="10" t="s">
         <v>33</v>
       </c>
@@ -3739,7 +3671,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="57" spans="1:5">
+    <row r="57" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A57" s="11" t="s">
         <v>112</v>
       </c>
@@ -3752,7 +3684,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="58" spans="1:5">
+    <row r="58" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A58" s="11" t="s">
         <v>34</v>
       </c>
@@ -3765,7 +3697,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="59" spans="1:5">
+    <row r="59" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A59" s="11" t="s">
         <v>200</v>
       </c>
@@ -3778,7 +3710,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="60" spans="1:5">
+    <row r="60" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A60" s="11" t="s">
         <v>106</v>
       </c>
@@ -3791,7 +3723,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="61" spans="1:5">
+    <row r="61" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A61" s="11" t="s">
         <v>148</v>
       </c>
@@ -3804,7 +3736,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="62" spans="1:5">
+    <row r="62" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A62" s="10" t="s">
         <v>121</v>
       </c>
@@ -3817,7 +3749,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="63" spans="1:5">
+    <row r="63" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A63" s="11" t="s">
         <v>122</v>
       </c>
@@ -3830,7 +3762,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="64" spans="1:5">
+    <row r="64" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A64" s="10" t="s">
         <v>26</v>
       </c>
@@ -3843,7 +3775,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="65" spans="1:5">
+    <row r="65" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A65" s="11" t="s">
         <v>27</v>
       </c>
@@ -3856,7 +3788,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="66" spans="1:5">
+    <row r="66" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A66" s="11" t="s">
         <v>49</v>
       </c>
@@ -3869,7 +3801,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="67" spans="1:5">
+    <row r="67" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A67" s="11" t="s">
         <v>48</v>
       </c>
@@ -3882,7 +3814,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="68" spans="1:5">
+    <row r="68" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A68" s="11" t="s">
         <v>41</v>
       </c>
@@ -3895,7 +3827,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="69" spans="1:5">
+    <row r="69" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A69" s="11" t="s">
         <v>74</v>
       </c>
@@ -3908,7 +3840,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="70" spans="1:5">
+    <row r="70" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A70" s="10" t="s">
         <v>142</v>
       </c>
@@ -3921,7 +3853,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="71" spans="1:5">
+    <row r="71" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A71" s="11" t="s">
         <v>80</v>
       </c>
@@ -3934,7 +3866,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="72" spans="1:5">
+    <row r="72" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A72" s="10" t="s">
         <v>211</v>
       </c>
@@ -3957,31 +3889,32 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:Q45"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:R46"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E21" sqref="E21"/>
+    <sheetView tabSelected="1" topLeftCell="A24" workbookViewId="0">
+      <selection activeCell="A46" sqref="A46"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="15.109375" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="15.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="4.88671875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="19.88671875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="22.44140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="20" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="27" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="19.44140625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12.109375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="44.33203125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="32.33203125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="5.44140625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="14.109375" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="34.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.109375" customWidth="1"/>
+    <col min="4" max="4" width="18.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.88671875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="22.44140625" customWidth="1"/>
+    <col min="7" max="7" width="20" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="27" customWidth="1"/>
+    <col min="9" max="9" width="19.44140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="44.33203125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="32.33203125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="5.44140625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="14.109375" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="34.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -3992,607 +3925,614 @@
         <v>23</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>1</v>
+        <v>272</v>
       </c>
       <c r="E1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="F1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="G1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="H1" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="I1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="J1" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="K1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="K1" s="2" t="s">
+      <c r="L1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="L1" s="2" t="s">
+      <c r="M1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="M1" s="2" t="s">
+      <c r="N1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="N1" s="2" t="s">
+      <c r="O1" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="O1" s="2" t="s">
+      <c r="P1" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="P1" s="2" t="s">
+      <c r="Q1" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="Q1" s="2" t="s">
+      <c r="R1" s="2" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="2" spans="1:17">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A2" s="3">
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>26</v>
+        <v>164</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>25</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E2" s="1"/>
+        <v>278</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>186</v>
+      </c>
       <c r="F2" s="1" t="s">
-        <v>27</v>
+        <v>188</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="H2" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="H2" s="1"/>
+      <c r="I2" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="I2" s="1" t="s">
+      <c r="J2" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="J2" s="1" t="s">
-        <v>28</v>
-      </c>
       <c r="K2" s="1" t="s">
-        <v>29</v>
+        <v>185</v>
       </c>
       <c r="L2" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="M2" s="1" t="s">
-        <v>30</v>
-      </c>
+        <v>187</v>
+      </c>
+      <c r="M2" s="1"/>
       <c r="N2" s="1" t="s">
-        <v>55</v>
+        <v>189</v>
       </c>
       <c r="O2" s="1"/>
       <c r="P2" s="1"/>
-      <c r="Q2" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="3" spans="1:17">
+      <c r="Q2" s="1"/>
+      <c r="R2" s="1"/>
+    </row>
+    <row r="3" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A3" s="3">
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>21</v>
+        <v>231</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>11</v>
+        <v>278</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="F3" s="15" t="s">
-        <v>10</v>
-      </c>
+        <v>232</v>
+      </c>
+      <c r="F3" s="1"/>
       <c r="G3" s="1" t="s">
-        <v>55</v>
+        <v>232</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>16</v>
+        <v>234</v>
       </c>
       <c r="I3" s="1" t="s">
+        <v>233</v>
+      </c>
+      <c r="J3" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="J3" s="6" t="s">
-        <v>62</v>
-      </c>
       <c r="K3" s="1" t="s">
-        <v>63</v>
+        <v>230</v>
       </c>
       <c r="L3" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="M3" s="1" t="s">
-        <v>61</v>
-      </c>
+        <v>237</v>
+      </c>
+      <c r="M3" s="1"/>
       <c r="N3" s="1" t="s">
-        <v>55</v>
+        <v>235</v>
       </c>
       <c r="O3" s="1"/>
       <c r="P3" s="1"/>
-      <c r="Q3" s="1" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="4" spans="1:17">
+      <c r="Q3" s="1"/>
+      <c r="R3" s="1" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A4" s="3">
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>20</v>
+        <v>85</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>14</v>
+        <v>278</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>15</v>
-      </c>
+        <v>86</v>
+      </c>
+      <c r="F4" s="1"/>
       <c r="G4" s="1" t="s">
-        <v>69</v>
+        <v>86</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>16</v>
+        <v>93</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>90</v>
+        <v>118</v>
       </c>
       <c r="J4" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="K4" s="1"/>
-      <c r="L4" s="1" t="s">
-        <v>71</v>
-      </c>
+        <v>88</v>
+      </c>
+      <c r="K4" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="L4" s="1"/>
       <c r="M4" s="1" t="s">
-        <v>17</v>
+        <v>55</v>
       </c>
       <c r="N4" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="O4" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="P4" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="Q4" s="1" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="5" spans="1:17">
+        <v>82</v>
+      </c>
+      <c r="O4" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="P4" s="1"/>
+      <c r="Q4" s="1"/>
+      <c r="R4" s="1" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A5" s="3">
         <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>33</v>
+        <v>164</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>25</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>8</v>
+        <v>275</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>43</v>
+        <v>165</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>34</v>
+        <v>166</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>55</v>
+        <v>165</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>16</v>
+        <v>169</v>
       </c>
       <c r="I5" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="J5" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="J5" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="K5" s="1"/>
+      <c r="K5" s="1" t="s">
+        <v>167</v>
+      </c>
       <c r="L5" s="1"/>
-      <c r="M5" s="1" t="s">
-        <v>36</v>
-      </c>
+      <c r="M5" s="1"/>
       <c r="N5" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="O5" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="P5" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="Q5" s="1" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="6" spans="1:17">
+        <v>170</v>
+      </c>
+      <c r="O5" s="1"/>
+      <c r="P5" s="1"/>
+      <c r="Q5" s="1"/>
+      <c r="R5" s="1" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="6" spans="1:18" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A6" s="3">
         <v>5</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>26</v>
+        <v>224</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>8</v>
+        <v>277</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="F6" s="15" t="s">
-        <v>41</v>
+        <v>122</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>40</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="H6" s="1" t="s">
-        <v>16</v>
-      </c>
+        <v>122</v>
+      </c>
+      <c r="H6" s="1"/>
       <c r="I6" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="J6" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="J6" s="1" t="s">
-        <v>44</v>
-      </c>
       <c r="K6" s="1" t="s">
-        <v>45</v>
+        <v>225</v>
       </c>
       <c r="L6" s="1" t="s">
-        <v>51</v>
+        <v>226</v>
       </c>
       <c r="M6" s="1" t="s">
-        <v>46</v>
+        <v>57</v>
       </c>
       <c r="N6" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="O6" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="P6" s="1"/>
-      <c r="Q6" s="1" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="7" spans="1:17">
+        <v>228</v>
+      </c>
+      <c r="O6" s="1"/>
+      <c r="P6" s="5" t="s">
+        <v>227</v>
+      </c>
+      <c r="Q6" s="1"/>
+      <c r="R6" s="1" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="7" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A7" s="3">
         <v>6</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>26</v>
+        <v>172</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>8</v>
+        <v>277</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="F7" s="1" t="s">
-        <v>48</v>
-      </c>
+        <v>122</v>
+      </c>
+      <c r="F7" s="1"/>
       <c r="G7" s="1" t="s">
-        <v>72</v>
+        <v>122</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>16</v>
+        <v>180</v>
       </c>
       <c r="I7" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="J7" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="J7" s="1" t="s">
-        <v>50</v>
-      </c>
       <c r="K7" s="1" t="s">
-        <v>53</v>
+        <v>181</v>
       </c>
       <c r="L7" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="M7" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="M7" s="1" t="s">
-        <v>46</v>
-      </c>
       <c r="N7" s="1" t="s">
-        <v>55</v>
+        <v>183</v>
       </c>
       <c r="O7" s="1"/>
       <c r="P7" s="1"/>
-      <c r="Q7" s="1" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="8" spans="1:17">
+      <c r="Q7" s="1"/>
+      <c r="R7" s="1" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="8" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A8" s="3">
         <v>7</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>26</v>
+        <v>172</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D8" s="1" t="s">
+        <v>277</v>
+      </c>
+      <c r="E8" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="E8" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="F8" s="1" t="s">
-        <v>49</v>
-      </c>
+      <c r="F8" s="1"/>
       <c r="G8" s="1" t="s">
-        <v>73</v>
+        <v>174</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>16</v>
+        <v>173</v>
       </c>
       <c r="I8" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="J8" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="J8" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="K8" s="1"/>
+      <c r="K8" s="1" t="s">
+        <v>176</v>
+      </c>
       <c r="L8" s="1" t="s">
-        <v>57</v>
+        <v>177</v>
       </c>
       <c r="M8" s="1" t="s">
-        <v>46</v>
+        <v>51</v>
       </c>
       <c r="N8" s="1" t="s">
-        <v>58</v>
+        <v>178</v>
       </c>
       <c r="O8" s="1"/>
       <c r="P8" s="1"/>
-      <c r="Q8" s="1" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="9" spans="1:17">
+      <c r="Q8" s="1"/>
+      <c r="R8" s="1" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="9" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A9" s="3">
         <v>8</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>26</v>
+        <v>121</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E9" s="1"/>
+        <v>277</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>122</v>
+      </c>
       <c r="F9" s="1" t="s">
-        <v>74</v>
+        <v>128</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>75</v>
+        <v>122</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>76</v>
+        <v>123</v>
       </c>
       <c r="I9" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="J9" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="J9" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="K9" s="1"/>
-      <c r="L9" s="1" t="s">
-        <v>71</v>
-      </c>
+      <c r="K9" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="L9" s="1"/>
       <c r="M9" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="N9" s="1"/>
+        <v>125</v>
+      </c>
+      <c r="N9" s="1" t="s">
+        <v>126</v>
+      </c>
       <c r="O9" s="1"/>
       <c r="P9" s="1"/>
-      <c r="Q9" s="1" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="10" spans="1:17">
+      <c r="Q9" s="1"/>
+      <c r="R9" s="1" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="10" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A10" s="3">
         <v>9</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>79</v>
+        <v>194</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>24</v>
       </c>
       <c r="D10" s="1" t="s">
+        <v>277</v>
+      </c>
+      <c r="E10" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="E10" s="1"/>
-      <c r="F10" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="G10" s="1"/>
-      <c r="H10" s="1" t="s">
+      <c r="F10" s="1"/>
+      <c r="G10" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="H10" s="1"/>
+      <c r="I10" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="I10" s="1" t="s">
+      <c r="J10" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="J10" s="1" t="s">
-        <v>83</v>
-      </c>
       <c r="K10" s="1" t="s">
-        <v>84</v>
+        <v>197</v>
       </c>
       <c r="L10" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="M10" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="N10" s="1"/>
+        <v>198</v>
+      </c>
+      <c r="M10" s="1"/>
+      <c r="N10" s="1" t="s">
+        <v>196</v>
+      </c>
       <c r="O10" s="1"/>
       <c r="P10" s="1"/>
       <c r="Q10" s="1"/>
-    </row>
-    <row r="11" spans="1:17">
+      <c r="R10" s="1" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="11" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A11" s="3">
         <v>10</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>85</v>
+        <v>139</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="E11" s="1"/>
-      <c r="F11" s="1" t="s">
-        <v>86</v>
-      </c>
+        <v>273</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F11" s="1"/>
       <c r="G11" s="1" t="s">
-        <v>93</v>
+        <v>41</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>118</v>
+        <v>140</v>
       </c>
       <c r="I11" s="1" t="s">
-        <v>88</v>
+        <v>16</v>
       </c>
       <c r="J11" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="K11" s="1"/>
-      <c r="L11" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="K11" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="L11" s="1"/>
+      <c r="M11" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="M11" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="N11" s="4" t="s">
-        <v>91</v>
+      <c r="N11" s="1" t="s">
+        <v>110</v>
       </c>
       <c r="O11" s="1"/>
       <c r="P11" s="1"/>
-      <c r="Q11" s="1" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="12" spans="1:17" ht="57.6">
+      <c r="Q11" s="1"/>
+      <c r="R11" s="1"/>
+    </row>
+    <row r="12" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A12" s="3">
         <v>11</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>94</v>
+        <v>242</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>24</v>
       </c>
       <c r="D12" s="1" t="s">
+        <v>273</v>
+      </c>
+      <c r="E12" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="E12" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="F12" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="G12" s="1"/>
-      <c r="H12" s="1" t="s">
-        <v>81</v>
-      </c>
+      <c r="F12" s="1"/>
+      <c r="G12" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="H12" s="1"/>
       <c r="I12" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="J12" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="J12" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="K12" s="5" t="s">
-        <v>98</v>
-      </c>
-      <c r="L12" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="M12" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="N12" s="1"/>
+      <c r="K12" s="1" t="s">
+        <v>243</v>
+      </c>
+      <c r="L12" s="1"/>
+      <c r="M12" s="1"/>
+      <c r="N12" s="1" t="s">
+        <v>244</v>
+      </c>
       <c r="O12" s="1"/>
       <c r="P12" s="1"/>
-      <c r="Q12" s="1" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="13" spans="1:17">
+      <c r="Q12" s="1"/>
+      <c r="R12" s="1" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="13" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A13" s="3">
         <v>12</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>101</v>
+        <v>20</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>24</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>102</v>
-      </c>
-      <c r="E13" s="1"/>
+        <v>273</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>14</v>
+      </c>
       <c r="F13" s="1" t="s">
-        <v>102</v>
-      </c>
-      <c r="G13" s="1"/>
+        <v>14</v>
+      </c>
+      <c r="G13" s="1" t="s">
+        <v>15</v>
+      </c>
       <c r="H13" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="I13" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="I13" s="1" t="s">
+      <c r="J13" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="J13" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="K13" s="1"/>
-      <c r="L13" s="1" t="s">
-        <v>57</v>
-      </c>
+      <c r="K13" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="L13" s="1"/>
       <c r="M13" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="N13" s="1"/>
-      <c r="O13" s="1"/>
-      <c r="P13" s="1"/>
+        <v>71</v>
+      </c>
+      <c r="N13" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="O13" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="P13" s="1" t="s">
+        <v>18</v>
+      </c>
       <c r="Q13" s="1" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="14" spans="1:17">
+        <v>19</v>
+      </c>
+      <c r="R13" s="1" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="14" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A14" s="3">
         <v>13</v>
       </c>
@@ -4603,1143 +4543,1242 @@
         <v>25</v>
       </c>
       <c r="D14" s="1" t="s">
+        <v>273</v>
+      </c>
+      <c r="E14" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="E14" s="1" t="s">
-        <v>111</v>
-      </c>
-      <c r="F14" s="15" t="s">
-        <v>106</v>
-      </c>
+      <c r="F14" s="1"/>
       <c r="G14" s="1" t="s">
-        <v>107</v>
+        <v>200</v>
       </c>
       <c r="H14" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="I14" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="I14" s="1" t="s">
+      <c r="J14" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="J14" s="1" t="s">
-        <v>108</v>
-      </c>
-      <c r="K14" s="1"/>
-      <c r="L14" s="1" t="s">
-        <v>55</v>
-      </c>
+      <c r="K14" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="L14" s="1"/>
       <c r="M14" s="1" t="s">
-        <v>110</v>
-      </c>
-      <c r="N14" s="1"/>
+        <v>71</v>
+      </c>
+      <c r="N14" s="1" t="s">
+        <v>203</v>
+      </c>
       <c r="O14" s="1"/>
       <c r="P14" s="1"/>
-      <c r="Q14" s="1" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="15" spans="1:17">
+      <c r="Q14" s="1"/>
+      <c r="R14" s="1" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="15" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A15" s="3">
         <v>14</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>33</v>
+        <v>142</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="D15" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>273</v>
+      </c>
+      <c r="E15" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="E15" s="1"/>
-      <c r="F15" s="1" t="s">
-        <v>112</v>
-      </c>
-      <c r="G15" s="1"/>
+      <c r="F15" s="1"/>
+      <c r="G15" s="1" t="s">
+        <v>80</v>
+      </c>
       <c r="H15" s="1" t="s">
-        <v>16</v>
+        <v>40</v>
       </c>
       <c r="I15" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="J15" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="J15" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="K15" s="1"/>
-      <c r="L15" s="1" t="s">
-        <v>57</v>
-      </c>
+      <c r="K15" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="L15" s="1"/>
       <c r="M15" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="N15" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="N15" s="1"/>
       <c r="O15" s="1"/>
       <c r="P15" s="1"/>
-      <c r="Q15" s="1" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="16" spans="1:17">
+      <c r="Q15" s="1"/>
+      <c r="R15" s="1"/>
+    </row>
+    <row r="16" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A16" s="3">
         <v>15</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>115</v>
+        <v>33</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>25</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>116</v>
-      </c>
-      <c r="E16" s="1"/>
-      <c r="F16" s="1" t="s">
-        <v>116</v>
-      </c>
-      <c r="G16" s="1"/>
-      <c r="H16" s="1" t="s">
-        <v>118</v>
-      </c>
+        <v>274</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F16" s="1"/>
+      <c r="G16" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="H16" s="1"/>
       <c r="I16" s="1" t="s">
-        <v>88</v>
+        <v>81</v>
       </c>
       <c r="J16" s="1" t="s">
-        <v>117</v>
-      </c>
-      <c r="K16" s="1"/>
+        <v>90</v>
+      </c>
+      <c r="K16" s="1" t="s">
+        <v>221</v>
+      </c>
       <c r="L16" s="1"/>
       <c r="M16" s="1" t="s">
-        <v>119</v>
-      </c>
-      <c r="N16" s="4" t="s">
-        <v>91</v>
+        <v>51</v>
+      </c>
+      <c r="N16" s="1" t="s">
+        <v>222</v>
       </c>
       <c r="O16" s="1"/>
       <c r="P16" s="1"/>
-      <c r="Q16" s="1" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="17" spans="1:17">
+      <c r="Q16" s="1"/>
+      <c r="R16" s="1" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="17" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A17" s="3">
         <v>16</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>121</v>
+        <v>25</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>122</v>
+        <v>274</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>128</v>
-      </c>
-      <c r="F17" s="1" t="s">
-        <v>122</v>
-      </c>
+        <v>264</v>
+      </c>
+      <c r="F17" s="1"/>
       <c r="G17" s="1" t="s">
-        <v>123</v>
-      </c>
-      <c r="H17" s="1" t="s">
-        <v>16</v>
-      </c>
+        <v>264</v>
+      </c>
+      <c r="H17" s="1"/>
       <c r="I17" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="J17" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="J17" s="1" t="s">
-        <v>124</v>
-      </c>
-      <c r="K17" s="1"/>
-      <c r="L17" s="1" t="s">
-        <v>125</v>
-      </c>
-      <c r="M17" s="1" t="s">
-        <v>126</v>
-      </c>
-      <c r="N17" s="1"/>
+      <c r="K17" s="1" t="s">
+        <v>265</v>
+      </c>
+      <c r="L17" s="1"/>
+      <c r="M17" s="1"/>
+      <c r="N17" s="1" t="s">
+        <v>266</v>
+      </c>
       <c r="O17" s="1"/>
       <c r="P17" s="1"/>
-      <c r="Q17" s="1" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="18" spans="1:17">
+      <c r="Q17" s="1"/>
+      <c r="R17" s="1" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="18" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A18" s="3">
         <v>17</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>129</v>
+        <v>115</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>8</v>
+        <v>274</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>132</v>
-      </c>
-      <c r="F18" s="15" t="s">
-        <v>130</v>
+        <v>205</v>
+      </c>
+      <c r="F18" s="1" t="s">
+        <v>206</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>131</v>
+        <v>205</v>
       </c>
       <c r="H18" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="I18" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="I18" s="1" t="s">
-        <v>90</v>
-      </c>
       <c r="J18" s="1" t="s">
-        <v>133</v>
+        <v>209</v>
       </c>
       <c r="K18" s="1" t="s">
-        <v>136</v>
-      </c>
-      <c r="L18" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="L18" s="1"/>
+      <c r="M18" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="M18" s="1" t="s">
-        <v>110</v>
-      </c>
-      <c r="N18" s="1"/>
-      <c r="O18" s="1"/>
+      <c r="N18" s="1" t="s">
+        <v>208</v>
+      </c>
+      <c r="O18" s="1" t="s">
+        <v>91</v>
+      </c>
       <c r="P18" s="1"/>
-      <c r="Q18" s="1" t="s">
-        <v>271</v>
-      </c>
-    </row>
-    <row r="19" spans="1:17">
+      <c r="Q18" s="1"/>
+      <c r="R18" s="1"/>
+    </row>
+    <row r="19" spans="1:18" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A19" s="3">
         <v>18</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="C19" s="1"/>
+        <v>94</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>24</v>
+      </c>
       <c r="D19" s="1" t="s">
+        <v>274</v>
+      </c>
+      <c r="E19" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="E19" s="1"/>
       <c r="F19" s="1" t="s">
-        <v>134</v>
-      </c>
-      <c r="G19" s="1"/>
-      <c r="H19" s="1" t="s">
-        <v>16</v>
-      </c>
+        <v>96</v>
+      </c>
+      <c r="G19" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="H19" s="1"/>
       <c r="I19" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="J19" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="J19" s="1" t="s">
-        <v>135</v>
-      </c>
       <c r="K19" s="1" t="s">
-        <v>137</v>
-      </c>
-      <c r="L19" s="1" t="s">
-        <v>66</v>
+        <v>97</v>
+      </c>
+      <c r="L19" s="5" t="s">
+        <v>98</v>
       </c>
       <c r="M19" s="1" t="s">
-        <v>110</v>
-      </c>
-      <c r="N19" s="1"/>
+        <v>55</v>
+      </c>
+      <c r="N19" s="1" t="s">
+        <v>100</v>
+      </c>
       <c r="O19" s="1"/>
       <c r="P19" s="1"/>
-      <c r="Q19" s="1" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="20" spans="1:17">
+      <c r="Q19" s="1"/>
+      <c r="R19" s="1" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="20" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A20" s="3">
         <v>19</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>139</v>
+        <v>26</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D20" s="1" t="s">
+        <v>274</v>
+      </c>
+      <c r="E20" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="E20" s="1"/>
-      <c r="F20" s="1" t="s">
-        <v>41</v>
-      </c>
+      <c r="F20" s="1"/>
       <c r="G20" s="1" t="s">
-        <v>140</v>
+        <v>74</v>
       </c>
       <c r="H20" s="1" t="s">
-        <v>16</v>
+        <v>75</v>
       </c>
       <c r="I20" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="J20" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="J20" s="1" t="s">
-        <v>141</v>
-      </c>
-      <c r="K20" s="1"/>
-      <c r="L20" s="1" t="s">
-        <v>55</v>
-      </c>
+      <c r="K20" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="L20" s="1"/>
       <c r="M20" s="1" t="s">
-        <v>110</v>
-      </c>
-      <c r="N20" s="1"/>
+        <v>71</v>
+      </c>
+      <c r="N20" s="1" t="s">
+        <v>17</v>
+      </c>
       <c r="O20" s="1"/>
       <c r="P20" s="1"/>
       <c r="Q20" s="1"/>
-    </row>
-    <row r="21" spans="1:17">
+      <c r="R20" s="1" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="21" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A21" s="3">
         <v>20</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>142</v>
+        <v>147</v>
       </c>
       <c r="C21" s="1" t="s">
         <v>24</v>
       </c>
       <c r="D21" s="1" t="s">
+        <v>274</v>
+      </c>
+      <c r="E21" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="E21" s="1"/>
       <c r="F21" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="G21" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="H21" s="1" t="s">
-        <v>81</v>
-      </c>
+        <v>159</v>
+      </c>
+      <c r="G21" s="15" t="s">
+        <v>270</v>
+      </c>
+      <c r="H21" s="1"/>
       <c r="I21" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="J21" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="J21" s="1" t="s">
-        <v>143</v>
-      </c>
-      <c r="K21" s="1"/>
+      <c r="K21" s="1" t="s">
+        <v>160</v>
+      </c>
       <c r="L21" s="1" t="s">
-        <v>55</v>
+        <v>161</v>
       </c>
       <c r="M21" s="1" t="s">
-        <v>110</v>
-      </c>
-      <c r="N21" s="1"/>
+        <v>66</v>
+      </c>
+      <c r="N21" s="1" t="s">
+        <v>162</v>
+      </c>
       <c r="O21" s="1"/>
       <c r="P21" s="1"/>
       <c r="Q21" s="1"/>
-    </row>
-    <row r="22" spans="1:17">
+      <c r="R21" s="1" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="22" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A22" s="3">
         <v>21</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>144</v>
+        <v>25</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D22" s="1" t="s">
+        <v>274</v>
+      </c>
+      <c r="E22" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="E22" s="1"/>
-      <c r="F22" s="1" t="s">
+      <c r="F22" s="1"/>
+      <c r="G22" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="G22" s="1"/>
-      <c r="H22" s="1" t="s">
+      <c r="H22" s="1"/>
+      <c r="I22" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="I22" s="1" t="s">
+      <c r="J22" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="J22" s="1" t="s">
-        <v>145</v>
-      </c>
-      <c r="K22" s="1"/>
-      <c r="L22" s="1" t="s">
-        <v>51</v>
-      </c>
+      <c r="K22" s="1" t="s">
+        <v>258</v>
+      </c>
+      <c r="L22" s="1"/>
       <c r="M22" s="1" t="s">
-        <v>110</v>
-      </c>
-      <c r="N22" s="1"/>
+        <v>125</v>
+      </c>
+      <c r="N22" s="1" t="s">
+        <v>259</v>
+      </c>
       <c r="O22" s="1"/>
       <c r="P22" s="1"/>
-      <c r="Q22" s="1" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="23" spans="1:17">
+      <c r="Q22" s="1"/>
+      <c r="R22" s="1" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="23" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A23" s="3">
         <v>22</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="C23" s="1" t="s">
         <v>24</v>
       </c>
       <c r="D23" s="1" t="s">
+        <v>274</v>
+      </c>
+      <c r="E23" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="E23" s="1" t="s">
-        <v>151</v>
-      </c>
-      <c r="F23" s="1" t="s">
-        <v>148</v>
-      </c>
-      <c r="G23" s="1"/>
-      <c r="H23" s="1" t="s">
+      <c r="F23" s="1"/>
+      <c r="G23" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="H23" s="1"/>
+      <c r="I23" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="I23" s="1" t="s">
+      <c r="J23" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="J23" s="1" t="s">
-        <v>149</v>
-      </c>
       <c r="K23" s="1" t="s">
-        <v>150</v>
+        <v>145</v>
       </c>
       <c r="L23" s="1"/>
       <c r="M23" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="N23" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="N23" s="1"/>
       <c r="O23" s="1"/>
       <c r="P23" s="1"/>
       <c r="Q23" s="1"/>
-    </row>
-    <row r="24" spans="1:17">
+      <c r="R23" s="1" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="24" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A24" s="3">
         <v>23</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>152</v>
+        <v>26</v>
       </c>
       <c r="C24" s="1" t="s">
         <v>25</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>153</v>
-      </c>
-      <c r="E24" s="1"/>
+        <v>276</v>
+      </c>
+      <c r="E24" s="1" t="s">
+        <v>8</v>
+      </c>
       <c r="F24" s="1" t="s">
-        <v>153</v>
-      </c>
-      <c r="G24" s="1"/>
+        <v>40</v>
+      </c>
+      <c r="G24" s="1" t="s">
+        <v>49</v>
+      </c>
       <c r="H24" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="I24" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="I24" s="1" t="s">
+      <c r="J24" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="J24" s="1" t="s">
-        <v>154</v>
-      </c>
       <c r="K24" s="1" t="s">
-        <v>155</v>
-      </c>
-      <c r="L24" s="1" t="s">
-        <v>156</v>
-      </c>
+        <v>56</v>
+      </c>
+      <c r="L24" s="1"/>
       <c r="M24" s="1" t="s">
-        <v>157</v>
-      </c>
-      <c r="N24" s="1"/>
-      <c r="O24" s="1"/>
+        <v>57</v>
+      </c>
+      <c r="N24" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="O24" s="1" t="s">
+        <v>58</v>
+      </c>
       <c r="P24" s="1"/>
-      <c r="Q24" s="1" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="25" spans="1:17">
+      <c r="Q24" s="1"/>
+      <c r="R24" s="1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="25" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A25" s="3">
         <v>24</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>147</v>
+        <v>26</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D25" s="1" t="s">
+        <v>276</v>
+      </c>
+      <c r="E25" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="E25" s="1" t="s">
-        <v>159</v>
-      </c>
-      <c r="F25" s="15" t="s">
-        <v>270</v>
-      </c>
-      <c r="G25" s="1"/>
+      <c r="F25" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="G25" s="1" t="s">
+        <v>48</v>
+      </c>
       <c r="H25" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="I25" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="I25" s="1" t="s">
+      <c r="J25" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="J25" s="1" t="s">
-        <v>160</v>
-      </c>
       <c r="K25" s="1" t="s">
-        <v>161</v>
+        <v>50</v>
       </c>
       <c r="L25" s="1" t="s">
-        <v>66</v>
+        <v>53</v>
       </c>
       <c r="M25" s="1" t="s">
-        <v>162</v>
-      </c>
-      <c r="N25" s="1"/>
-      <c r="O25" s="1"/>
+        <v>51</v>
+      </c>
+      <c r="N25" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="O25" s="1" t="s">
+        <v>55</v>
+      </c>
       <c r="P25" s="1"/>
-      <c r="Q25" s="1" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="26" spans="1:17">
+      <c r="Q25" s="1"/>
+      <c r="R25" s="1" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="26" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A26" s="3">
         <v>25</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>164</v>
+        <v>33</v>
       </c>
       <c r="C26" s="1" t="s">
         <v>25</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>165</v>
+        <v>279</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>166</v>
+        <v>8</v>
       </c>
       <c r="F26" s="1" t="s">
-        <v>165</v>
+        <v>43</v>
       </c>
       <c r="G26" s="1" t="s">
-        <v>169</v>
+        <v>34</v>
       </c>
       <c r="H26" s="1" t="s">
-        <v>168</v>
+        <v>55</v>
       </c>
       <c r="I26" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="J26" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="J26" s="1" t="s">
-        <v>167</v>
-      </c>
-      <c r="K26" s="1"/>
+      <c r="K26" s="1" t="s">
+        <v>35</v>
+      </c>
       <c r="L26" s="1"/>
-      <c r="M26" s="1" t="s">
-        <v>170</v>
-      </c>
-      <c r="N26" s="1"/>
-      <c r="O26" s="1"/>
-      <c r="P26" s="1"/>
+      <c r="M26" s="1"/>
+      <c r="N26" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="O26" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="P26" s="1" t="s">
+        <v>37</v>
+      </c>
       <c r="Q26" s="1" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="27" spans="1:17">
+        <v>38</v>
+      </c>
+      <c r="R26" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="27" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A27" s="3">
         <v>26</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>172</v>
+        <v>101</v>
       </c>
       <c r="C27" s="1" t="s">
         <v>24</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E27" s="1"/>
-      <c r="F27" s="1" t="s">
-        <v>174</v>
-      </c>
+        <v>279</v>
+      </c>
+      <c r="E27" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="F27" s="1"/>
       <c r="G27" s="1" t="s">
-        <v>173</v>
-      </c>
-      <c r="H27" s="1" t="s">
-        <v>175</v>
-      </c>
+        <v>102</v>
+      </c>
+      <c r="H27" s="1"/>
       <c r="I27" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="J27" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="J27" s="1" t="s">
-        <v>176</v>
-      </c>
       <c r="K27" s="1" t="s">
-        <v>177</v>
-      </c>
-      <c r="L27" s="1" t="s">
-        <v>51</v>
-      </c>
+        <v>103</v>
+      </c>
+      <c r="L27" s="1"/>
       <c r="M27" s="1" t="s">
-        <v>178</v>
-      </c>
-      <c r="N27" s="1"/>
+        <v>57</v>
+      </c>
+      <c r="N27" s="1" t="s">
+        <v>104</v>
+      </c>
       <c r="O27" s="1"/>
       <c r="P27" s="1"/>
-      <c r="Q27" s="1" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="28" spans="1:17">
+      <c r="Q27" s="1"/>
+      <c r="R27" s="1" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="28" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A28" s="3">
         <v>27</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>172</v>
+        <v>33</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>122</v>
-      </c>
-      <c r="E28" s="1"/>
+        <v>279</v>
+      </c>
+      <c r="E28" s="1" t="s">
+        <v>8</v>
+      </c>
       <c r="F28" s="1" t="s">
-        <v>122</v>
-      </c>
-      <c r="G28" s="1" t="s">
-        <v>180</v>
+        <v>111</v>
+      </c>
+      <c r="G28" s="15" t="s">
+        <v>106</v>
       </c>
       <c r="H28" s="1" t="s">
-        <v>175</v>
+        <v>107</v>
       </c>
       <c r="I28" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="J28" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="J28" s="1" t="s">
-        <v>181</v>
-      </c>
       <c r="K28" s="1" t="s">
-        <v>182</v>
-      </c>
-      <c r="L28" s="1" t="s">
-        <v>51</v>
-      </c>
+        <v>108</v>
+      </c>
+      <c r="L28" s="1"/>
       <c r="M28" s="1" t="s">
-        <v>183</v>
-      </c>
-      <c r="N28" s="1"/>
+        <v>55</v>
+      </c>
+      <c r="N28" s="1" t="s">
+        <v>110</v>
+      </c>
       <c r="O28" s="1"/>
       <c r="P28" s="1"/>
-      <c r="Q28" s="1" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="29" spans="1:17">
+      <c r="Q28" s="1"/>
+      <c r="R28" s="1" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="29" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A29" s="3">
         <v>28</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>164</v>
+        <v>129</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>186</v>
+        <v>279</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>188</v>
+        <v>8</v>
       </c>
       <c r="F29" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="G29" s="1"/>
+        <v>132</v>
+      </c>
+      <c r="G29" s="15" t="s">
+        <v>130</v>
+      </c>
       <c r="H29" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="I29" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="I29" s="1" t="s">
+      <c r="J29" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="J29" s="1" t="s">
-        <v>185</v>
-      </c>
       <c r="K29" s="1" t="s">
-        <v>187</v>
-      </c>
-      <c r="L29" s="1"/>
+        <v>133</v>
+      </c>
+      <c r="L29" s="1" t="s">
+        <v>136</v>
+      </c>
       <c r="M29" s="1" t="s">
-        <v>189</v>
-      </c>
-      <c r="N29" s="1"/>
+        <v>71</v>
+      </c>
+      <c r="N29" s="1" t="s">
+        <v>110</v>
+      </c>
       <c r="O29" s="1"/>
       <c r="P29" s="1"/>
       <c r="Q29" s="1"/>
-    </row>
-    <row r="30" spans="1:17">
+      <c r="R29" s="1" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="30" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A30" s="3">
         <v>29</v>
       </c>
-      <c r="B30" s="1" t="s">
+      <c r="B30" s="7" t="s">
+        <v>214</v>
+      </c>
+      <c r="C30" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="C30" s="1" t="s">
-        <v>25</v>
-      </c>
       <c r="D30" s="1" t="s">
+        <v>279</v>
+      </c>
+      <c r="E30" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="E30" s="1"/>
-      <c r="F30" s="7" t="s">
-        <v>190</v>
-      </c>
-      <c r="G30" s="1"/>
-      <c r="H30" s="1" t="s">
+      <c r="F30" s="1" t="s">
+        <v>216</v>
+      </c>
+      <c r="G30" s="7" t="s">
+        <v>215</v>
+      </c>
+      <c r="H30" s="1"/>
+      <c r="I30" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="I30" s="1" t="s">
+      <c r="J30" s="7" t="s">
         <v>90</v>
       </c>
-      <c r="J30" s="1" t="s">
-        <v>191</v>
-      </c>
-      <c r="K30" s="1"/>
-      <c r="L30" s="1" t="s">
-        <v>192</v>
-      </c>
-      <c r="M30" s="1"/>
-      <c r="N30" s="1"/>
+      <c r="K30" s="7" t="s">
+        <v>217</v>
+      </c>
+      <c r="L30" s="7" t="s">
+        <v>218</v>
+      </c>
+      <c r="M30" s="7" t="s">
+        <v>125</v>
+      </c>
+      <c r="N30" s="7" t="s">
+        <v>219</v>
+      </c>
       <c r="O30" s="1"/>
       <c r="P30" s="1"/>
-      <c r="Q30" s="1" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="31" spans="1:17">
+      <c r="Q30" s="1"/>
+      <c r="R30" s="1" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="31" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A31" s="3">
         <v>30</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>194</v>
-      </c>
-      <c r="C31" s="1" t="s">
-        <v>24</v>
-      </c>
+        <v>20</v>
+      </c>
+      <c r="C31" s="1"/>
       <c r="D31" s="1" t="s">
+        <v>280</v>
+      </c>
+      <c r="E31" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="E31" s="1"/>
-      <c r="F31" s="1" t="s">
-        <v>195</v>
-      </c>
-      <c r="G31" s="1"/>
-      <c r="H31" s="1" t="s">
-        <v>81</v>
-      </c>
+      <c r="F31" s="1"/>
+      <c r="G31" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="H31" s="1"/>
       <c r="I31" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="J31" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="J31" s="1" t="s">
-        <v>197</v>
-      </c>
       <c r="K31" s="1" t="s">
-        <v>198</v>
-      </c>
-      <c r="L31" s="1"/>
+        <v>135</v>
+      </c>
+      <c r="L31" s="1" t="s">
+        <v>137</v>
+      </c>
       <c r="M31" s="1" t="s">
-        <v>196</v>
-      </c>
-      <c r="N31" s="1"/>
+        <v>66</v>
+      </c>
+      <c r="N31" s="1" t="s">
+        <v>110</v>
+      </c>
       <c r="O31" s="1"/>
       <c r="P31" s="1"/>
-      <c r="Q31" s="1" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="32" spans="1:17">
+      <c r="Q31" s="1"/>
+      <c r="R31" s="1" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="32" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A32" s="3">
         <v>31</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
       <c r="C32" s="1" t="s">
         <v>25</v>
       </c>
       <c r="D32" s="1" t="s">
+        <v>280</v>
+      </c>
+      <c r="E32" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="E32" s="1"/>
       <c r="F32" s="1" t="s">
-        <v>200</v>
-      </c>
-      <c r="G32" s="1" t="s">
-        <v>201</v>
+        <v>42</v>
+      </c>
+      <c r="G32" s="15" t="s">
+        <v>41</v>
       </c>
       <c r="H32" s="1" t="s">
-        <v>81</v>
+        <v>55</v>
       </c>
       <c r="I32" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="J32" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="J32" s="1" t="s">
-        <v>202</v>
-      </c>
-      <c r="K32" s="1"/>
+      <c r="K32" s="1" t="s">
+        <v>44</v>
+      </c>
       <c r="L32" s="1" t="s">
-        <v>71</v>
+        <v>45</v>
       </c>
       <c r="M32" s="1" t="s">
-        <v>203</v>
-      </c>
-      <c r="N32" s="1"/>
-      <c r="O32" s="1"/>
-      <c r="P32" s="1"/>
-      <c r="Q32" s="1" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="33" spans="1:17">
+        <v>51</v>
+      </c>
+      <c r="N32" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="O32" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="P32" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="Q32" s="1"/>
+      <c r="R32" s="1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="33" spans="1:18" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A33" s="3">
         <v>32</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>115</v>
+        <v>246</v>
       </c>
       <c r="C33" s="1" t="s">
         <v>25</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>205</v>
+        <v>281</v>
       </c>
       <c r="E33" s="1" t="s">
-        <v>206</v>
-      </c>
-      <c r="F33" s="1" t="s">
-        <v>205</v>
-      </c>
+        <v>186</v>
+      </c>
+      <c r="F33" s="1"/>
       <c r="G33" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="H33" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="I33" s="1" t="s">
+        <v>247</v>
+      </c>
+      <c r="H33" s="1"/>
+      <c r="I33" s="1"/>
+      <c r="J33" s="1" t="s">
         <v>209</v>
       </c>
-      <c r="J33" s="1" t="s">
-        <v>207</v>
-      </c>
-      <c r="K33" s="1"/>
-      <c r="L33" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="M33" s="1" t="s">
-        <v>208</v>
-      </c>
+      <c r="K33" s="1" t="s">
+        <v>248</v>
+      </c>
+      <c r="L33" s="5" t="s">
+        <v>250</v>
+      </c>
+      <c r="M33" s="1"/>
       <c r="N33" s="1" t="s">
-        <v>91</v>
+        <v>249</v>
       </c>
       <c r="O33" s="1"/>
       <c r="P33" s="1"/>
       <c r="Q33" s="1"/>
-    </row>
-    <row r="34" spans="1:17">
+      <c r="R33" s="1" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="34" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A34" s="3">
         <v>33</v>
       </c>
-      <c r="B34" s="7" t="s">
-        <v>214</v>
-      </c>
-      <c r="C34" s="7" t="s">
+      <c r="B34" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C34" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="D34" s="7" t="s">
+      <c r="D34" s="1" t="s">
+        <v>281</v>
+      </c>
+      <c r="E34" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="E34" s="1" t="s">
-        <v>216</v>
-      </c>
-      <c r="F34" s="7" t="s">
-        <v>215</v>
-      </c>
-      <c r="G34" s="1"/>
-      <c r="H34" s="7" t="s">
+      <c r="F34" s="1"/>
+      <c r="G34" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="H34" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="I34" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="I34" s="7" t="s">
+      <c r="J34" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="J34" s="7" t="s">
-        <v>217</v>
-      </c>
-      <c r="K34" s="7" t="s">
-        <v>218</v>
-      </c>
-      <c r="L34" s="7" t="s">
-        <v>125</v>
-      </c>
-      <c r="M34" s="7" t="s">
-        <v>219</v>
-      </c>
-      <c r="N34" s="1"/>
-      <c r="O34" s="1"/>
+      <c r="K34" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="L34" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="M34" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="N34" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="O34" s="1" t="s">
+        <v>55</v>
+      </c>
       <c r="P34" s="1"/>
-      <c r="Q34" s="1" t="s">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="35" spans="1:17">
+      <c r="Q34" s="1"/>
+      <c r="R34" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="35" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A35" s="3">
         <v>34</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>33</v>
+        <v>231</v>
       </c>
       <c r="C35" s="1" t="s">
         <v>25</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E35" s="1"/>
-      <c r="F35" s="1" t="s">
-        <v>148</v>
-      </c>
-      <c r="G35" s="1"/>
+        <v>282</v>
+      </c>
+      <c r="E35" s="1" t="s">
+        <v>232</v>
+      </c>
+      <c r="F35" s="1"/>
+      <c r="G35" s="1" t="s">
+        <v>232</v>
+      </c>
       <c r="H35" s="1" t="s">
-        <v>81</v>
+        <v>240</v>
       </c>
       <c r="I35" s="1" t="s">
+        <v>233</v>
+      </c>
+      <c r="J35" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="J35" s="1" t="s">
-        <v>221</v>
-      </c>
-      <c r="K35" s="1"/>
-      <c r="L35" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="M35" s="1" t="s">
-        <v>222</v>
-      </c>
-      <c r="N35" s="1"/>
+      <c r="K35" s="1" t="s">
+        <v>238</v>
+      </c>
+      <c r="L35" s="1"/>
+      <c r="M35" s="1"/>
+      <c r="N35" s="1" t="s">
+        <v>239</v>
+      </c>
       <c r="O35" s="1"/>
       <c r="P35" s="1"/>
-      <c r="Q35" s="1" t="s">
-        <v>223</v>
-      </c>
-    </row>
-    <row r="36" spans="1:17" ht="57.6">
+      <c r="Q35" s="1"/>
+      <c r="R35" s="1" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="36" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A36" s="3">
         <v>35</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>224</v>
+        <v>33</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>122</v>
-      </c>
-      <c r="E36" s="1"/>
-      <c r="F36" s="1" t="s">
-        <v>122</v>
-      </c>
-      <c r="G36" s="1"/>
-      <c r="H36" s="1" t="s">
-        <v>81</v>
-      </c>
+        <v>283</v>
+      </c>
+      <c r="E36" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="F36" s="1"/>
+      <c r="G36" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="H36" s="1"/>
       <c r="I36" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="J36" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="J36" s="1" t="s">
-        <v>225</v>
-      </c>
       <c r="K36" s="1" t="s">
-        <v>226</v>
-      </c>
-      <c r="L36" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="L36" s="1"/>
+      <c r="M36" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="M36" s="1" t="s">
-        <v>228</v>
-      </c>
-      <c r="N36" s="1"/>
-      <c r="O36" s="5" t="s">
-        <v>227</v>
-      </c>
+      <c r="N36" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="O36" s="1"/>
       <c r="P36" s="1"/>
-      <c r="Q36" s="1" t="s">
-        <v>229</v>
-      </c>
-    </row>
-    <row r="37" spans="1:17">
+      <c r="Q36" s="1"/>
+      <c r="R36" s="1" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="37" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A37" s="3">
         <v>36</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>231</v>
+        <v>25</v>
       </c>
       <c r="C37" s="1" t="s">
         <v>25</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>232</v>
-      </c>
-      <c r="E37" s="1"/>
-      <c r="F37" s="1" t="s">
-        <v>232</v>
-      </c>
+        <v>283</v>
+      </c>
+      <c r="E37" s="1" t="s">
+        <v>261</v>
+      </c>
+      <c r="F37" s="1"/>
       <c r="G37" s="1" t="s">
-        <v>234</v>
-      </c>
-      <c r="H37" s="1" t="s">
-        <v>233</v>
-      </c>
+        <v>261</v>
+      </c>
+      <c r="H37" s="1"/>
       <c r="I37" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="J37" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="J37" s="1" t="s">
-        <v>230</v>
-      </c>
       <c r="K37" s="1" t="s">
-        <v>237</v>
+        <v>113</v>
       </c>
       <c r="L37" s="1"/>
-      <c r="M37" s="1" t="s">
-        <v>235</v>
-      </c>
-      <c r="N37" s="1"/>
+      <c r="M37" s="1"/>
+      <c r="N37" s="1" t="s">
+        <v>268</v>
+      </c>
       <c r="O37" s="1"/>
       <c r="P37" s="1"/>
-      <c r="Q37" s="1" t="s">
-        <v>236</v>
-      </c>
-    </row>
-    <row r="38" spans="1:17">
+      <c r="Q37" s="1"/>
+      <c r="R37" s="1" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="38" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A38" s="3">
         <v>37</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>231</v>
+        <v>79</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>232</v>
-      </c>
-      <c r="E38" s="1"/>
-      <c r="F38" s="1" t="s">
-        <v>232</v>
-      </c>
+        <v>283</v>
+      </c>
+      <c r="E38" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F38" s="1"/>
       <c r="G38" s="1" t="s">
-        <v>240</v>
-      </c>
-      <c r="H38" s="1" t="s">
-        <v>233</v>
-      </c>
+        <v>80</v>
+      </c>
+      <c r="H38" s="1"/>
       <c r="I38" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="J38" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="J38" s="1" t="s">
-        <v>238</v>
-      </c>
-      <c r="K38" s="1"/>
-      <c r="L38" s="1"/>
+      <c r="K38" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="L38" s="1" t="s">
+        <v>84</v>
+      </c>
       <c r="M38" s="1" t="s">
-        <v>239</v>
-      </c>
-      <c r="N38" s="1"/>
+        <v>51</v>
+      </c>
+      <c r="N38" s="1" t="s">
+        <v>82</v>
+      </c>
       <c r="O38" s="1"/>
       <c r="P38" s="1"/>
-      <c r="Q38" s="1" t="s">
-        <v>241</v>
-      </c>
-    </row>
-    <row r="39" spans="1:17">
+      <c r="Q38" s="1"/>
+      <c r="R38" s="1"/>
+    </row>
+    <row r="39" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A39" s="3">
         <v>38</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>242</v>
+        <v>25</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D39" s="1" t="s">
+        <v>283</v>
+      </c>
+      <c r="E39" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="E39" s="1"/>
-      <c r="F39" s="1" t="s">
-        <v>195</v>
-      </c>
-      <c r="G39" s="1"/>
-      <c r="H39" s="1" t="s">
+      <c r="F39" s="1"/>
+      <c r="G39" s="7" t="s">
+        <v>190</v>
+      </c>
+      <c r="H39" s="1"/>
+      <c r="I39" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="I39" s="1" t="s">
+      <c r="J39" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="J39" s="1" t="s">
-        <v>243</v>
-      </c>
-      <c r="K39" s="1"/>
+      <c r="K39" s="1" t="s">
+        <v>191</v>
+      </c>
       <c r="L39" s="1"/>
       <c r="M39" s="1" t="s">
-        <v>244</v>
+        <v>192</v>
       </c>
       <c r="N39" s="1"/>
       <c r="O39" s="1"/>
       <c r="P39" s="1"/>
-      <c r="Q39" s="1" t="s">
-        <v>245</v>
-      </c>
-    </row>
-    <row r="40" spans="1:17" ht="43.2">
+      <c r="Q39" s="1"/>
+      <c r="R39" s="1" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="40" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A40" s="3">
         <v>39</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>246</v>
+        <v>25</v>
       </c>
       <c r="C40" s="1" t="s">
         <v>25</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>186</v>
-      </c>
-      <c r="E40" s="1"/>
-      <c r="F40" s="1" t="s">
-        <v>247</v>
-      </c>
-      <c r="G40" s="1"/>
+        <v>283</v>
+      </c>
+      <c r="E40" s="1" t="s">
+        <v>261</v>
+      </c>
+      <c r="F40" s="1"/>
+      <c r="G40" s="1" t="s">
+        <v>261</v>
+      </c>
       <c r="H40" s="1"/>
       <c r="I40" s="1" t="s">
-        <v>209</v>
+        <v>81</v>
       </c>
       <c r="J40" s="1" t="s">
-        <v>248</v>
-      </c>
-      <c r="K40" s="5" t="s">
-        <v>250</v>
+        <v>90</v>
+      </c>
+      <c r="K40" s="1" t="s">
+        <v>262</v>
       </c>
       <c r="L40" s="1"/>
       <c r="M40" s="1" t="s">
-        <v>249</v>
+        <v>71</v>
       </c>
       <c r="N40" s="1"/>
       <c r="O40" s="1"/>
       <c r="P40" s="1"/>
-      <c r="Q40" s="1" t="s">
-        <v>251</v>
-      </c>
-    </row>
-    <row r="41" spans="1:17" ht="43.2">
+      <c r="Q40" s="1"/>
+      <c r="R40" s="1" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="41" spans="1:18" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A41" s="3">
         <v>40</v>
       </c>
@@ -5750,212 +5789,292 @@
         <v>25</v>
       </c>
       <c r="D41" s="1" t="s">
+        <v>283</v>
+      </c>
+      <c r="E41" s="1" t="s">
         <v>252</v>
       </c>
-      <c r="E41" s="1"/>
-      <c r="F41" s="1" t="s">
+      <c r="F41" s="1"/>
+      <c r="G41" s="1" t="s">
         <v>252</v>
       </c>
-      <c r="G41" s="1"/>
-      <c r="H41" s="1" t="s">
+      <c r="H41" s="1"/>
+      <c r="I41" s="1" t="s">
         <v>253</v>
       </c>
-      <c r="I41" s="1" t="s">
+      <c r="J41" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="J41" s="1" t="s">
+      <c r="K41" s="1" t="s">
         <v>254</v>
       </c>
-      <c r="K41" s="5" t="s">
+      <c r="L41" s="5" t="s">
         <v>255</v>
       </c>
-      <c r="L41" s="1"/>
-      <c r="M41" s="1" t="s">
+      <c r="M41" s="1"/>
+      <c r="N41" s="1" t="s">
         <v>256</v>
       </c>
-      <c r="N41" s="1"/>
       <c r="O41" s="1"/>
       <c r="P41" s="1"/>
-      <c r="Q41" s="1" t="s">
+      <c r="Q41" s="1"/>
+      <c r="R41" s="1" t="s">
         <v>257</v>
       </c>
     </row>
-    <row r="42" spans="1:17">
+    <row r="42" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A42" s="3">
         <v>41</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>25</v>
+        <v>115</v>
       </c>
       <c r="C42" s="1" t="s">
         <v>25</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E42" s="1"/>
-      <c r="F42" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="G42" s="1"/>
-      <c r="H42" s="1" t="s">
-        <v>16</v>
-      </c>
+        <v>283</v>
+      </c>
+      <c r="E42" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="F42" s="1"/>
+      <c r="G42" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="H42" s="1"/>
       <c r="I42" s="1" t="s">
-        <v>90</v>
+        <v>118</v>
       </c>
       <c r="J42" s="1" t="s">
-        <v>258</v>
-      </c>
-      <c r="K42" s="1"/>
-      <c r="L42" s="1" t="s">
-        <v>125</v>
-      </c>
-      <c r="M42" s="1" t="s">
-        <v>259</v>
-      </c>
-      <c r="N42" s="1"/>
-      <c r="O42" s="1"/>
+        <v>88</v>
+      </c>
+      <c r="K42" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="L42" s="1"/>
+      <c r="M42" s="1"/>
+      <c r="N42" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="O42" s="4" t="s">
+        <v>91</v>
+      </c>
       <c r="P42" s="1"/>
-      <c r="Q42" s="1" t="s">
-        <v>260</v>
-      </c>
-    </row>
-    <row r="43" spans="1:17">
+      <c r="Q42" s="1"/>
+      <c r="R42" s="1" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="43" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A43" s="3">
         <v>42</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>25</v>
+        <v>147</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>261</v>
-      </c>
-      <c r="E43" s="1"/>
+        <v>283</v>
+      </c>
+      <c r="E43" s="1" t="s">
+        <v>8</v>
+      </c>
       <c r="F43" s="1" t="s">
-        <v>261</v>
-      </c>
-      <c r="G43" s="1"/>
-      <c r="H43" s="1" t="s">
-        <v>81</v>
-      </c>
+        <v>151</v>
+      </c>
+      <c r="G43" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="H43" s="1"/>
       <c r="I43" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="J43" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="J43" s="1" t="s">
-        <v>262</v>
-      </c>
-      <c r="K43" s="1"/>
+      <c r="K43" s="1" t="s">
+        <v>149</v>
+      </c>
       <c r="L43" s="1" t="s">
-        <v>71</v>
+        <v>150</v>
       </c>
       <c r="M43" s="1"/>
-      <c r="N43" s="1"/>
+      <c r="N43" s="1" t="s">
+        <v>110</v>
+      </c>
       <c r="O43" s="1"/>
       <c r="P43" s="1"/>
-      <c r="Q43" s="1" t="s">
-        <v>263</v>
-      </c>
-    </row>
-    <row r="44" spans="1:17">
+      <c r="Q43" s="1"/>
+      <c r="R43" s="1"/>
+    </row>
+    <row r="44" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A44" s="3">
         <v>43</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>25</v>
+        <v>152</v>
       </c>
       <c r="C44" s="1" t="s">
         <v>25</v>
       </c>
       <c r="D44" s="1" t="s">
-        <v>264</v>
-      </c>
-      <c r="E44" s="1"/>
-      <c r="F44" s="1" t="s">
-        <v>264</v>
-      </c>
-      <c r="G44" s="1"/>
-      <c r="H44" s="1" t="s">
-        <v>81</v>
-      </c>
+        <v>284</v>
+      </c>
+      <c r="E44" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="F44" s="1"/>
+      <c r="G44" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="H44" s="1"/>
       <c r="I44" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="J44" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="J44" s="1" t="s">
-        <v>265</v>
-      </c>
-      <c r="K44" s="1"/>
-      <c r="L44" s="1"/>
+      <c r="K44" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="L44" s="1" t="s">
+        <v>155</v>
+      </c>
       <c r="M44" s="1" t="s">
-        <v>266</v>
-      </c>
-      <c r="N44" s="1"/>
+        <v>156</v>
+      </c>
+      <c r="N44" s="1" t="s">
+        <v>157</v>
+      </c>
       <c r="O44" s="1"/>
       <c r="P44" s="1"/>
-      <c r="Q44" s="1" t="s">
-        <v>267</v>
-      </c>
-    </row>
-    <row r="45" spans="1:17">
+      <c r="Q44" s="1"/>
+      <c r="R44" s="1" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="45" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A45" s="3">
         <v>44</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D45" s="1" t="s">
-        <v>261</v>
-      </c>
-      <c r="E45" s="1"/>
+        <v>284</v>
+      </c>
+      <c r="E45" s="1" t="s">
+        <v>11</v>
+      </c>
       <c r="F45" s="1" t="s">
-        <v>261</v>
-      </c>
-      <c r="G45" s="1"/>
+        <v>10</v>
+      </c>
+      <c r="G45" s="15" t="s">
+        <v>10</v>
+      </c>
       <c r="H45" s="1" t="s">
-        <v>81</v>
+        <v>55</v>
       </c>
       <c r="I45" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="J45" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="J45" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="K45" s="1"/>
-      <c r="L45" s="1"/>
+      <c r="K45" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="L45" s="1" t="s">
+        <v>63</v>
+      </c>
       <c r="M45" s="1" t="s">
-        <v>268</v>
-      </c>
-      <c r="N45" s="1"/>
-      <c r="O45" s="1"/>
+        <v>57</v>
+      </c>
+      <c r="N45" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="O45" s="1" t="s">
+        <v>55</v>
+      </c>
       <c r="P45" s="1"/>
-      <c r="Q45" t="s">
-        <v>269</v>
+      <c r="Q45" s="1"/>
+      <c r="R45" s="1" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="46" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A46" s="16">
+        <v>45</v>
+      </c>
+      <c r="B46" s="7" t="s">
+        <v>285</v>
+      </c>
+      <c r="C46" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="D46" s="7" t="s">
+        <v>274</v>
+      </c>
+      <c r="E46" s="7" t="s">
+        <v>290</v>
+      </c>
+      <c r="F46" s="1" t="s">
+        <v>291</v>
+      </c>
+      <c r="G46" s="1"/>
+      <c r="H46" s="7" t="s">
+        <v>286</v>
+      </c>
+      <c r="I46" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="J46" s="7" t="s">
+        <v>90</v>
+      </c>
+      <c r="K46" s="7" t="s">
+        <v>287</v>
+      </c>
+      <c r="L46" s="1"/>
+      <c r="M46" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="N46" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="O46" s="1"/>
+      <c r="P46" s="1" t="s">
+        <v>288</v>
+      </c>
+      <c r="Q46" s="1"/>
+      <c r="R46" s="1" t="s">
+        <v>289</v>
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:R45" xr:uid="{00000000-0009-0000-0000-000001000000}"/>
   <hyperlinks>
-    <hyperlink ref="Q3" r:id="rId1"/>
+    <hyperlink ref="R45" r:id="rId1" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId2"/>
+  <pageSetup orientation="landscape" r:id="rId2"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C30" sqref="C30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Updated Lease Property details
</commit_message>
<xml_diff>
--- a/ASRProps-Final.xlsx
+++ b/ASRProps-Final.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/a063b81c7d42b926/Documents/ASR-Props/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="8" documentId="11_B65B585BC469815E41FBBAE2ED8C4BDFAD7A2CD5" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{71E0437A-9D52-4D41-A90A-0F30A2340369}"/>
+  <xr:revisionPtr revIDLastSave="11" documentId="11_B65B585BC469815E41FBBAE2ED8C4BDFAD7A2CD5" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{636F438D-66CD-4D50-845E-A1450F337620}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -18,7 +18,7 @@
     <sheet name="Home" sheetId="4" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Property Details'!$A$1:$R$45</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Property Details'!$A$1:$R$46</definedName>
   </definedNames>
   <calcPr calcId="124519"/>
   <pivotCaches>
@@ -251,9 +251,6 @@
     <t>NORTH</t>
   </si>
   <si>
-    <t>Plot No 272 *</t>
-  </si>
-  <si>
     <t>Plot No 399</t>
   </si>
   <si>
@@ -916,6 +913,9 @@
   </si>
   <si>
     <t>left from Wipro Circle</t>
+  </si>
+  <si>
+    <t>Plot No 273</t>
   </si>
 </sst>
 </file>
@@ -2693,7 +2693,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light"/>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -2745,7 +2745,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -2970,27 +2970,27 @@
   <sheetData>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="8" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="B3" s="13" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="9" t="s">
+        <v>209</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>208</v>
+      </c>
+      <c r="E4" s="3" t="s">
         <v>210</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>88</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>90</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>209</v>
-      </c>
-      <c r="E4" s="3" t="s">
-        <v>211</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
@@ -3008,7 +3008,7 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" s="11" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="B6" s="14"/>
       <c r="C6" s="14">
@@ -3021,7 +3021,7 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" s="11" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="B7" s="14"/>
       <c r="C7" s="14">
@@ -3034,7 +3034,7 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" s="11" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="B8" s="14"/>
       <c r="C8" s="14">
@@ -3047,7 +3047,7 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" s="11" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B9" s="14"/>
       <c r="C9" s="14">
@@ -3060,7 +3060,7 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" s="11" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="B10" s="14"/>
       <c r="C10" s="14">
@@ -3073,7 +3073,7 @@
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" s="10" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="B11" s="14"/>
       <c r="C11" s="14">
@@ -3086,7 +3086,7 @@
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" s="11" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="B12" s="14"/>
       <c r="C12" s="14">
@@ -3099,7 +3099,7 @@
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" s="10" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B13" s="14"/>
       <c r="C13" s="14">
@@ -3112,7 +3112,7 @@
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" s="11" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B14" s="14"/>
       <c r="C14" s="14">
@@ -3125,7 +3125,7 @@
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" s="11" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B15" s="14"/>
       <c r="C15" s="14">
@@ -3138,7 +3138,7 @@
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" s="10" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B16" s="14"/>
       <c r="C16" s="14">
@@ -3151,7 +3151,7 @@
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" s="11" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B17" s="14"/>
       <c r="C17" s="14">
@@ -3164,7 +3164,7 @@
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" s="10" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="B18" s="14"/>
       <c r="C18" s="14">
@@ -3177,7 +3177,7 @@
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19" s="11" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="B19" s="14"/>
       <c r="C19" s="14">
@@ -3190,7 +3190,7 @@
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20" s="10" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B20" s="14"/>
       <c r="C20" s="14">
@@ -3203,7 +3203,7 @@
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21" s="11" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B21" s="14"/>
       <c r="C21" s="14">
@@ -3216,7 +3216,7 @@
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22" s="10" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B22" s="14"/>
       <c r="C22" s="14">
@@ -3229,7 +3229,7 @@
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A23" s="11" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B23" s="14"/>
       <c r="C23" s="14">
@@ -3255,7 +3255,7 @@
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A25" s="11" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B25" s="14"/>
       <c r="C25" s="14">
@@ -3281,7 +3281,7 @@
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A27" s="10" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B27" s="14"/>
       <c r="C27" s="14">
@@ -3294,7 +3294,7 @@
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A28" s="11" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B28" s="14"/>
       <c r="C28" s="14">
@@ -3307,7 +3307,7 @@
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A29" s="10" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B29" s="14"/>
       <c r="C29" s="14">
@@ -3320,7 +3320,7 @@
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A30" s="11" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B30" s="14"/>
       <c r="C30" s="14">
@@ -3333,7 +3333,7 @@
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A31" s="10" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B31" s="14">
         <v>1</v>
@@ -3348,7 +3348,7 @@
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A32" s="11" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B32" s="14">
         <v>1</v>
@@ -3361,7 +3361,7 @@
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A33" s="11" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B33" s="14"/>
       <c r="C33" s="14"/>
@@ -3374,7 +3374,7 @@
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A34" s="10" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B34" s="14">
         <v>1</v>
@@ -3387,7 +3387,7 @@
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A35" s="11" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B35" s="14">
         <v>1</v>
@@ -3400,7 +3400,7 @@
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A36" s="10" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B36" s="14"/>
       <c r="C36" s="14">
@@ -3413,7 +3413,7 @@
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A37" s="11" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B37" s="14"/>
       <c r="C37" s="14">
@@ -3426,7 +3426,7 @@
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A38" s="10" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="B38" s="14"/>
       <c r="C38" s="14">
@@ -3439,7 +3439,7 @@
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A39" s="11" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B39" s="14"/>
       <c r="C39" s="14">
@@ -3452,7 +3452,7 @@
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A40" s="10" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="B40" s="14"/>
       <c r="C40" s="14">
@@ -3465,7 +3465,7 @@
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A41" s="11" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="B41" s="14"/>
       <c r="C41" s="14">
@@ -3478,7 +3478,7 @@
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A42" s="10" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B42" s="14"/>
       <c r="C42" s="14">
@@ -3504,7 +3504,7 @@
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A44" s="11" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B44" s="14"/>
       <c r="C44" s="14">
@@ -3543,7 +3543,7 @@
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A47" s="10" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B47" s="14"/>
       <c r="C47" s="14">
@@ -3556,7 +3556,7 @@
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A48" s="11" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="B48" s="14"/>
       <c r="C48" s="14">
@@ -3569,7 +3569,7 @@
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A49" s="11" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B49" s="14"/>
       <c r="C49" s="14">
@@ -3582,7 +3582,7 @@
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A50" s="10" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B50" s="14"/>
       <c r="C50" s="14">
@@ -3608,7 +3608,7 @@
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A52" s="10" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="B52" s="14"/>
       <c r="C52" s="14"/>
@@ -3621,7 +3621,7 @@
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A53" s="11" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="B53" s="14"/>
       <c r="C53" s="14"/>
@@ -3634,7 +3634,7 @@
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A54" s="10" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="B54" s="14"/>
       <c r="C54" s="14">
@@ -3647,7 +3647,7 @@
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A55" s="11" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="B55" s="14"/>
       <c r="C55" s="14">
@@ -3673,7 +3673,7 @@
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A57" s="11" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B57" s="14"/>
       <c r="C57" s="14">
@@ -3699,7 +3699,7 @@
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A59" s="11" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="B59" s="14"/>
       <c r="C59" s="14">
@@ -3712,7 +3712,7 @@
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A60" s="11" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B60" s="14"/>
       <c r="C60" s="14">
@@ -3725,7 +3725,7 @@
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A61" s="11" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B61" s="14"/>
       <c r="C61" s="14">
@@ -3738,7 +3738,7 @@
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A62" s="10" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B62" s="14"/>
       <c r="C62" s="14">
@@ -3751,7 +3751,7 @@
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A63" s="11" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B63" s="14"/>
       <c r="C63" s="14">
@@ -3829,7 +3829,7 @@
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A69" s="11" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B69" s="14"/>
       <c r="C69" s="14">
@@ -3842,7 +3842,7 @@
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A70" s="10" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B70" s="14"/>
       <c r="C70" s="14">
@@ -3855,7 +3855,7 @@
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A71" s="11" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B71" s="14"/>
       <c r="C71" s="14">
@@ -3868,7 +3868,7 @@
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A72" s="10" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B72" s="14">
         <v>2</v>
@@ -3892,8 +3892,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:R46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A24" workbookViewId="0">
-      <selection activeCell="A46" sqref="A46"/>
+    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="G46" sqref="G46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="15.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3925,7 +3925,7 @@
         <v>23</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="E1" s="2" t="s">
         <v>1</v>
@@ -3943,7 +3943,7 @@
         <v>3</v>
       </c>
       <c r="J1" s="2" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="K1" s="2" t="s">
         <v>4</v>
@@ -3975,19 +3975,19 @@
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>25</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="G2" s="1" t="s">
         <v>34</v>
@@ -3997,17 +3997,17 @@
         <v>16</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="L2" s="1" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="M2" s="1"/>
       <c r="N2" s="1" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="O2" s="1"/>
       <c r="P2" s="1"/>
@@ -4019,45 +4019,45 @@
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>25</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="F3" s="1"/>
       <c r="G3" s="1" t="s">
+        <v>231</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>233</v>
+      </c>
+      <c r="I3" s="1" t="s">
         <v>232</v>
       </c>
-      <c r="H3" s="1" t="s">
-        <v>234</v>
-      </c>
-      <c r="I3" s="1" t="s">
-        <v>233</v>
-      </c>
       <c r="J3" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="K3" s="1" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="L3" s="1" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="M3" s="1"/>
       <c r="N3" s="1" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="O3" s="1"/>
       <c r="P3" s="1"/>
       <c r="Q3" s="1"/>
       <c r="R3" s="1" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.3">
@@ -4065,47 +4065,47 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>25</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F4" s="1"/>
       <c r="G4" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="J4" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="K4" s="1" t="s">
         <v>86</v>
-      </c>
-      <c r="H4" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="I4" s="1" t="s">
-        <v>118</v>
-      </c>
-      <c r="J4" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="K4" s="1" t="s">
-        <v>87</v>
       </c>
       <c r="L4" s="1"/>
       <c r="M4" s="1" t="s">
         <v>55</v>
       </c>
       <c r="N4" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="O4" s="4" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="P4" s="1"/>
       <c r="Q4" s="1"/>
       <c r="R4" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.3">
@@ -4113,45 +4113,45 @@
         <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>25</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="E5" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="F5" s="1" t="s">
         <v>165</v>
       </c>
-      <c r="F5" s="1" t="s">
+      <c r="G5" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="I5" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="J5" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="K5" s="1" t="s">
         <v>166</v>
-      </c>
-      <c r="G5" s="1" t="s">
-        <v>165</v>
-      </c>
-      <c r="H5" s="1" t="s">
-        <v>169</v>
-      </c>
-      <c r="I5" s="1" t="s">
-        <v>168</v>
-      </c>
-      <c r="J5" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="K5" s="1" t="s">
-        <v>167</v>
       </c>
       <c r="L5" s="1"/>
       <c r="M5" s="1"/>
       <c r="N5" s="1" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="O5" s="1"/>
       <c r="P5" s="1"/>
       <c r="Q5" s="1"/>
       <c r="R5" s="1" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="6" spans="1:18" ht="57.6" x14ac:dyDescent="0.3">
@@ -4159,49 +4159,49 @@
         <v>5</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>24</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="F6" s="1" t="s">
         <v>40</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="H6" s="1"/>
       <c r="I6" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="J6" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="K6" s="1" t="s">
+        <v>224</v>
+      </c>
+      <c r="L6" s="1" t="s">
         <v>225</v>
-      </c>
-      <c r="L6" s="1" t="s">
-        <v>226</v>
       </c>
       <c r="M6" s="1" t="s">
         <v>57</v>
       </c>
       <c r="N6" s="1" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="O6" s="1"/>
       <c r="P6" s="5" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="Q6" s="1"/>
       <c r="R6" s="1" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.3">
@@ -4209,47 +4209,47 @@
         <v>6</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>24</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="F7" s="1"/>
       <c r="G7" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="H7" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="I7" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="J7" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="K7" s="1" t="s">
         <v>180</v>
       </c>
-      <c r="I7" s="1" t="s">
-        <v>175</v>
-      </c>
-      <c r="J7" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="K7" s="1" t="s">
+      <c r="L7" s="1" t="s">
         <v>181</v>
-      </c>
-      <c r="L7" s="1" t="s">
-        <v>182</v>
       </c>
       <c r="M7" s="1" t="s">
         <v>51</v>
       </c>
       <c r="N7" s="1" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="O7" s="1"/>
       <c r="P7" s="1"/>
       <c r="Q7" s="1"/>
       <c r="R7" s="1" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.3">
@@ -4257,47 +4257,47 @@
         <v>7</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>24</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="E8" s="1" t="s">
         <v>8</v>
       </c>
       <c r="F8" s="1"/>
       <c r="G8" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="H8" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="I8" s="1" t="s">
         <v>174</v>
       </c>
-      <c r="H8" s="1" t="s">
-        <v>173</v>
-      </c>
-      <c r="I8" s="1" t="s">
+      <c r="J8" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="K8" s="1" t="s">
         <v>175</v>
       </c>
-      <c r="J8" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="K8" s="1" t="s">
+      <c r="L8" s="1" t="s">
         <v>176</v>
-      </c>
-      <c r="L8" s="1" t="s">
-        <v>177</v>
       </c>
       <c r="M8" s="1" t="s">
         <v>51</v>
       </c>
       <c r="N8" s="1" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="O8" s="1"/>
       <c r="P8" s="1"/>
       <c r="Q8" s="1"/>
       <c r="R8" s="1" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.3">
@@ -4305,47 +4305,47 @@
         <v>8</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>24</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="E9" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="H9" s="1" t="s">
         <v>122</v>
-      </c>
-      <c r="F9" s="1" t="s">
-        <v>128</v>
-      </c>
-      <c r="G9" s="1" t="s">
-        <v>122</v>
-      </c>
-      <c r="H9" s="1" t="s">
-        <v>123</v>
       </c>
       <c r="I9" s="1" t="s">
         <v>16</v>
       </c>
       <c r="J9" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="K9" s="1" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="L9" s="1"/>
       <c r="M9" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="N9" s="1" t="s">
         <v>125</v>
-      </c>
-      <c r="N9" s="1" t="s">
-        <v>126</v>
       </c>
       <c r="O9" s="1"/>
       <c r="P9" s="1"/>
       <c r="Q9" s="1"/>
       <c r="R9" s="1" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.3">
@@ -4353,43 +4353,43 @@
         <v>9</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>24</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="E10" s="1" t="s">
         <v>8</v>
       </c>
       <c r="F10" s="1"/>
       <c r="G10" s="1" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="H10" s="1"/>
       <c r="I10" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="J10" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="K10" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="L10" s="1" t="s">
         <v>197</v>
-      </c>
-      <c r="L10" s="1" t="s">
-        <v>198</v>
       </c>
       <c r="M10" s="1"/>
       <c r="N10" s="1" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="O10" s="1"/>
       <c r="P10" s="1"/>
       <c r="Q10" s="1"/>
       <c r="R10" s="1" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="11" spans="1:18" x14ac:dyDescent="0.3">
@@ -4397,13 +4397,13 @@
         <v>10</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>24</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="E11" s="1" t="s">
         <v>8</v>
@@ -4413,23 +4413,23 @@
         <v>41</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="I11" s="1" t="s">
         <v>16</v>
       </c>
       <c r="J11" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="K11" s="1" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="L11" s="1"/>
       <c r="M11" s="1" t="s">
         <v>55</v>
       </c>
       <c r="N11" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="O11" s="1"/>
       <c r="P11" s="1"/>
@@ -4441,41 +4441,41 @@
         <v>11</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>24</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="E12" s="1" t="s">
         <v>8</v>
       </c>
       <c r="F12" s="1"/>
       <c r="G12" s="1" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="H12" s="1"/>
       <c r="I12" s="1" t="s">
         <v>16</v>
       </c>
       <c r="J12" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="K12" s="1" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="L12" s="1"/>
       <c r="M12" s="1"/>
       <c r="N12" s="1" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="O12" s="1"/>
       <c r="P12" s="1"/>
       <c r="Q12" s="1"/>
       <c r="R12" s="1" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="13" spans="1:18" x14ac:dyDescent="0.3">
@@ -4489,7 +4489,7 @@
         <v>24</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="E13" s="1" t="s">
         <v>14</v>
@@ -4507,7 +4507,7 @@
         <v>16</v>
       </c>
       <c r="J13" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="K13" s="1" t="s">
         <v>70</v>
@@ -4543,39 +4543,39 @@
         <v>25</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="E14" s="1" t="s">
         <v>8</v>
       </c>
       <c r="F14" s="1"/>
       <c r="G14" s="1" t="s">
+        <v>199</v>
+      </c>
+      <c r="H14" s="1" t="s">
         <v>200</v>
       </c>
-      <c r="H14" s="1" t="s">
+      <c r="I14" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="J14" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="K14" s="1" t="s">
         <v>201</v>
-      </c>
-      <c r="I14" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="J14" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="K14" s="1" t="s">
-        <v>202</v>
       </c>
       <c r="L14" s="1"/>
       <c r="M14" s="1" t="s">
         <v>71</v>
       </c>
       <c r="N14" s="1" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="O14" s="1"/>
       <c r="P14" s="1"/>
       <c r="Q14" s="1"/>
       <c r="R14" s="1" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="15" spans="1:18" x14ac:dyDescent="0.3">
@@ -4583,39 +4583,39 @@
         <v>14</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>24</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="E15" s="1" t="s">
         <v>8</v>
       </c>
       <c r="F15" s="1"/>
       <c r="G15" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="H15" s="1" t="s">
         <v>40</v>
       </c>
       <c r="I15" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="J15" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="K15" s="1" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="L15" s="1"/>
       <c r="M15" s="1" t="s">
         <v>55</v>
       </c>
       <c r="N15" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="O15" s="1"/>
       <c r="P15" s="1"/>
@@ -4633,37 +4633,37 @@
         <v>25</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="E16" s="1" t="s">
         <v>8</v>
       </c>
       <c r="F16" s="1"/>
       <c r="G16" s="1" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="H16" s="1"/>
       <c r="I16" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="J16" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="K16" s="1" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="L16" s="1"/>
       <c r="M16" s="1" t="s">
         <v>51</v>
       </c>
       <c r="N16" s="1" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="O16" s="1"/>
       <c r="P16" s="1"/>
       <c r="Q16" s="1"/>
       <c r="R16" s="1" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="17" spans="1:18" x14ac:dyDescent="0.3">
@@ -4677,35 +4677,35 @@
         <v>25</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="F17" s="1"/>
       <c r="G17" s="1" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="H17" s="1"/>
       <c r="I17" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="J17" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="K17" s="1" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="L17" s="1"/>
       <c r="M17" s="1"/>
       <c r="N17" s="1" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="O17" s="1"/>
       <c r="P17" s="1"/>
       <c r="Q17" s="1"/>
       <c r="R17" s="1" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="18" spans="1:18" x14ac:dyDescent="0.3">
@@ -4713,22 +4713,22 @@
         <v>17</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C18" s="1" t="s">
         <v>25</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="E18" s="1" t="s">
+        <v>204</v>
+      </c>
+      <c r="F18" s="1" t="s">
         <v>205</v>
       </c>
-      <c r="F18" s="1" t="s">
-        <v>206</v>
-      </c>
       <c r="G18" s="1" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="H18" s="1" t="s">
         <v>40</v>
@@ -4737,20 +4737,20 @@
         <v>16</v>
       </c>
       <c r="J18" s="1" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="K18" s="1" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="L18" s="1"/>
       <c r="M18" s="1" t="s">
         <v>71</v>
       </c>
       <c r="N18" s="1" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="O18" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="P18" s="1"/>
       <c r="Q18" s="1"/>
@@ -4761,47 +4761,47 @@
         <v>18</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C19" s="1" t="s">
         <v>24</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="E19" s="1" t="s">
         <v>8</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="G19" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="H19" s="1"/>
       <c r="I19" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="J19" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="K19" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="L19" s="5" t="s">
         <v>97</v>
-      </c>
-      <c r="L19" s="5" t="s">
-        <v>98</v>
       </c>
       <c r="M19" s="1" t="s">
         <v>55</v>
       </c>
       <c r="N19" s="1" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="O19" s="1"/>
       <c r="P19" s="1"/>
       <c r="Q19" s="1"/>
       <c r="R19" s="1" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="20" spans="1:18" x14ac:dyDescent="0.3">
@@ -4815,26 +4815,26 @@
         <v>25</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="E20" s="1" t="s">
         <v>8</v>
       </c>
       <c r="F20" s="1"/>
       <c r="G20" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="H20" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="H20" s="1" t="s">
+      <c r="I20" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="I20" s="1" t="s">
+      <c r="J20" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="K20" s="1" t="s">
         <v>76</v>
-      </c>
-      <c r="J20" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="K20" s="1" t="s">
-        <v>77</v>
       </c>
       <c r="L20" s="1"/>
       <c r="M20" s="1" t="s">
@@ -4847,7 +4847,7 @@
       <c r="P20" s="1"/>
       <c r="Q20" s="1"/>
       <c r="R20" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="21" spans="1:18" x14ac:dyDescent="0.3">
@@ -4855,47 +4855,47 @@
         <v>20</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C21" s="1" t="s">
         <v>24</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="E21" s="1" t="s">
         <v>8</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="G21" s="15" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="H21" s="1"/>
       <c r="I21" s="1" t="s">
         <v>16</v>
       </c>
       <c r="J21" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="K21" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="L21" s="1" t="s">
         <v>160</v>
-      </c>
-      <c r="L21" s="1" t="s">
-        <v>161</v>
       </c>
       <c r="M21" s="1" t="s">
         <v>66</v>
       </c>
       <c r="N21" s="1" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="O21" s="1"/>
       <c r="P21" s="1"/>
       <c r="Q21" s="1"/>
       <c r="R21" s="1" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="22" spans="1:18" x14ac:dyDescent="0.3">
@@ -4909,37 +4909,37 @@
         <v>25</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="E22" s="1" t="s">
         <v>8</v>
       </c>
       <c r="F22" s="1"/>
       <c r="G22" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="H22" s="1"/>
       <c r="I22" s="1" t="s">
         <v>16</v>
       </c>
       <c r="J22" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="K22" s="1" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="L22" s="1"/>
       <c r="M22" s="1" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="N22" s="1" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="O22" s="1"/>
       <c r="P22" s="1"/>
       <c r="Q22" s="1"/>
       <c r="R22" s="1" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="23" spans="1:18" x14ac:dyDescent="0.3">
@@ -4947,43 +4947,43 @@
         <v>22</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C23" s="1" t="s">
         <v>24</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="E23" s="1" t="s">
         <v>8</v>
       </c>
       <c r="F23" s="1"/>
       <c r="G23" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="H23" s="1"/>
       <c r="I23" s="1" t="s">
         <v>16</v>
       </c>
       <c r="J23" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="K23" s="1" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="L23" s="1"/>
       <c r="M23" s="1" t="s">
         <v>51</v>
       </c>
       <c r="N23" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="O23" s="1"/>
       <c r="P23" s="1"/>
       <c r="Q23" s="1"/>
       <c r="R23" s="1" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="24" spans="1:18" x14ac:dyDescent="0.3">
@@ -4997,7 +4997,7 @@
         <v>25</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="E24" s="1" t="s">
         <v>8</v>
@@ -5009,13 +5009,13 @@
         <v>49</v>
       </c>
       <c r="H24" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="I24" s="1" t="s">
         <v>16</v>
       </c>
       <c r="J24" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="K24" s="1" t="s">
         <v>56</v>
@@ -5047,7 +5047,7 @@
         <v>25</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="E25" s="1" t="s">
         <v>8</v>
@@ -5059,13 +5059,13 @@
         <v>48</v>
       </c>
       <c r="H25" s="1" t="s">
-        <v>72</v>
+        <v>291</v>
       </c>
       <c r="I25" s="1" t="s">
         <v>16</v>
       </c>
       <c r="J25" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="K25" s="1" t="s">
         <v>50</v>
@@ -5099,7 +5099,7 @@
         <v>25</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="E26" s="1" t="s">
         <v>8</v>
@@ -5117,7 +5117,7 @@
         <v>16</v>
       </c>
       <c r="J26" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="K26" s="1" t="s">
         <v>35</v>
@@ -5145,43 +5145,43 @@
         <v>26</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C27" s="1" t="s">
         <v>24</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="F27" s="1"/>
       <c r="G27" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="H27" s="1"/>
       <c r="I27" s="1" t="s">
         <v>16</v>
       </c>
       <c r="J27" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="K27" s="1" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="L27" s="1"/>
       <c r="M27" s="1" t="s">
         <v>57</v>
       </c>
       <c r="N27" s="1" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="O27" s="1"/>
       <c r="P27" s="1"/>
       <c r="Q27" s="1"/>
       <c r="R27" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="28" spans="1:18" x14ac:dyDescent="0.3">
@@ -5195,41 +5195,41 @@
         <v>25</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="E28" s="1" t="s">
         <v>8</v>
       </c>
       <c r="F28" s="1" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="G28" s="15" t="s">
+        <v>105</v>
+      </c>
+      <c r="H28" s="1" t="s">
         <v>106</v>
       </c>
-      <c r="H28" s="1" t="s">
+      <c r="I28" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="J28" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="K28" s="1" t="s">
         <v>107</v>
-      </c>
-      <c r="I28" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="J28" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="K28" s="1" t="s">
-        <v>108</v>
       </c>
       <c r="L28" s="1"/>
       <c r="M28" s="1" t="s">
         <v>55</v>
       </c>
       <c r="N28" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="O28" s="1"/>
       <c r="P28" s="1"/>
       <c r="Q28" s="1"/>
       <c r="R28" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="29" spans="1:18" x14ac:dyDescent="0.3">
@@ -5237,49 +5237,49 @@
         <v>28</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C29" s="1" t="s">
         <v>24</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="E29" s="1" t="s">
         <v>8</v>
       </c>
       <c r="F29" s="1" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="G29" s="15" t="s">
+        <v>129</v>
+      </c>
+      <c r="H29" s="1" t="s">
         <v>130</v>
-      </c>
-      <c r="H29" s="1" t="s">
-        <v>131</v>
       </c>
       <c r="I29" s="1" t="s">
         <v>16</v>
       </c>
       <c r="J29" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="K29" s="1" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="L29" s="1" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="M29" s="1" t="s">
         <v>71</v>
       </c>
       <c r="N29" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="O29" s="1"/>
       <c r="P29" s="1"/>
       <c r="Q29" s="1"/>
       <c r="R29" s="1" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="30" spans="1:18" x14ac:dyDescent="0.3">
@@ -5287,47 +5287,47 @@
         <v>29</v>
       </c>
       <c r="B30" s="7" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="C30" s="7" t="s">
         <v>25</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="E30" s="7" t="s">
         <v>8</v>
       </c>
       <c r="F30" s="1" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="G30" s="7" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="H30" s="1"/>
       <c r="I30" s="7" t="s">
         <v>16</v>
       </c>
       <c r="J30" s="7" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="K30" s="7" t="s">
+        <v>216</v>
+      </c>
+      <c r="L30" s="7" t="s">
         <v>217</v>
       </c>
-      <c r="L30" s="7" t="s">
+      <c r="M30" s="7" t="s">
+        <v>124</v>
+      </c>
+      <c r="N30" s="7" t="s">
         <v>218</v>
-      </c>
-      <c r="M30" s="7" t="s">
-        <v>125</v>
-      </c>
-      <c r="N30" s="7" t="s">
-        <v>219</v>
       </c>
       <c r="O30" s="1"/>
       <c r="P30" s="1"/>
       <c r="Q30" s="1"/>
       <c r="R30" s="1" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="31" spans="1:18" x14ac:dyDescent="0.3">
@@ -5339,39 +5339,39 @@
       </c>
       <c r="C31" s="1"/>
       <c r="D31" s="1" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="E31" s="1" t="s">
         <v>8</v>
       </c>
       <c r="F31" s="1"/>
       <c r="G31" s="1" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="H31" s="1"/>
       <c r="I31" s="1" t="s">
         <v>16</v>
       </c>
       <c r="J31" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="K31" s="1" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="L31" s="1" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="M31" s="1" t="s">
         <v>66</v>
       </c>
       <c r="N31" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="O31" s="1"/>
       <c r="P31" s="1"/>
       <c r="Q31" s="1"/>
       <c r="R31" s="1" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="32" spans="1:18" x14ac:dyDescent="0.3">
@@ -5385,7 +5385,7 @@
         <v>25</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="E32" s="1" t="s">
         <v>8</v>
@@ -5403,7 +5403,7 @@
         <v>16</v>
       </c>
       <c r="J32" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="K32" s="1" t="s">
         <v>44</v>
@@ -5433,41 +5433,41 @@
         <v>32</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="C33" s="1" t="s">
         <v>25</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="E33" s="1" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="F33" s="1"/>
       <c r="G33" s="1" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="H33" s="1"/>
       <c r="I33" s="1"/>
       <c r="J33" s="1" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="K33" s="1" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="L33" s="5" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="M33" s="1"/>
       <c r="N33" s="1" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="O33" s="1"/>
       <c r="P33" s="1"/>
       <c r="Q33" s="1"/>
       <c r="R33" s="1" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
     </row>
     <row r="34" spans="1:18" x14ac:dyDescent="0.3">
@@ -5481,7 +5481,7 @@
         <v>25</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="E34" s="1" t="s">
         <v>8</v>
@@ -5497,7 +5497,7 @@
         <v>16</v>
       </c>
       <c r="J34" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="K34" s="1" t="s">
         <v>28</v>
@@ -5525,43 +5525,43 @@
         <v>34</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="C35" s="1" t="s">
         <v>25</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="E35" s="1" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="F35" s="1"/>
       <c r="G35" s="1" t="s">
+        <v>231</v>
+      </c>
+      <c r="H35" s="1" t="s">
+        <v>239</v>
+      </c>
+      <c r="I35" s="1" t="s">
         <v>232</v>
       </c>
-      <c r="H35" s="1" t="s">
-        <v>240</v>
-      </c>
-      <c r="I35" s="1" t="s">
-        <v>233</v>
-      </c>
       <c r="J35" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="K35" s="1" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="L35" s="1"/>
       <c r="M35" s="1"/>
       <c r="N35" s="1" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="O35" s="1"/>
       <c r="P35" s="1"/>
       <c r="Q35" s="1"/>
       <c r="R35" s="1" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="36" spans="1:18" x14ac:dyDescent="0.3">
@@ -5575,37 +5575,37 @@
         <v>25</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="E36" s="7" t="s">
         <v>8</v>
       </c>
       <c r="F36" s="1"/>
       <c r="G36" s="1" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="H36" s="1"/>
       <c r="I36" s="1" t="s">
         <v>16</v>
       </c>
       <c r="J36" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="K36" s="1" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="L36" s="1"/>
       <c r="M36" s="1" t="s">
         <v>57</v>
       </c>
       <c r="N36" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="O36" s="1"/>
       <c r="P36" s="1"/>
       <c r="Q36" s="1"/>
       <c r="R36" s="1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="37" spans="1:18" x14ac:dyDescent="0.3">
@@ -5619,35 +5619,35 @@
         <v>25</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="E37" s="1" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="F37" s="1"/>
       <c r="G37" s="1" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="H37" s="1"/>
       <c r="I37" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="J37" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="K37" s="1" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="L37" s="1"/>
       <c r="M37" s="1"/>
       <c r="N37" s="1" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="O37" s="1"/>
       <c r="P37" s="1"/>
       <c r="Q37" s="1"/>
       <c r="R37" s="1" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
     </row>
     <row r="38" spans="1:18" x14ac:dyDescent="0.3">
@@ -5655,39 +5655,39 @@
         <v>37</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C38" s="1" t="s">
         <v>24</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="E38" s="1" t="s">
         <v>8</v>
       </c>
       <c r="F38" s="1"/>
       <c r="G38" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="H38" s="1"/>
       <c r="I38" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="J38" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="K38" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="L38" s="1" t="s">
         <v>83</v>
-      </c>
-      <c r="L38" s="1" t="s">
-        <v>84</v>
       </c>
       <c r="M38" s="1" t="s">
         <v>51</v>
       </c>
       <c r="N38" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="O38" s="1"/>
       <c r="P38" s="1"/>
@@ -5705,35 +5705,35 @@
         <v>25</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="E39" s="1" t="s">
         <v>8</v>
       </c>
       <c r="F39" s="1"/>
       <c r="G39" s="7" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="H39" s="1"/>
       <c r="I39" s="1" t="s">
         <v>16</v>
       </c>
       <c r="J39" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="K39" s="1" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="L39" s="1"/>
       <c r="M39" s="1" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="N39" s="1"/>
       <c r="O39" s="1"/>
       <c r="P39" s="1"/>
       <c r="Q39" s="1"/>
       <c r="R39" s="1" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="40" spans="1:18" x14ac:dyDescent="0.3">
@@ -5747,24 +5747,24 @@
         <v>25</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="E40" s="1" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="F40" s="1"/>
       <c r="G40" s="1" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="H40" s="1"/>
       <c r="I40" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="J40" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="K40" s="1" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="L40" s="1"/>
       <c r="M40" s="1" t="s">
@@ -5775,7 +5775,7 @@
       <c r="P40" s="1"/>
       <c r="Q40" s="1"/>
       <c r="R40" s="1" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
     </row>
     <row r="41" spans="1:18" ht="43.2" x14ac:dyDescent="0.3">
@@ -5789,37 +5789,37 @@
         <v>25</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="E41" s="1" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="F41" s="1"/>
       <c r="G41" s="1" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="H41" s="1"/>
       <c r="I41" s="1" t="s">
+        <v>252</v>
+      </c>
+      <c r="J41" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="K41" s="1" t="s">
         <v>253</v>
       </c>
-      <c r="J41" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="K41" s="1" t="s">
+      <c r="L41" s="5" t="s">
         <v>254</v>
-      </c>
-      <c r="L41" s="5" t="s">
-        <v>255</v>
       </c>
       <c r="M41" s="1"/>
       <c r="N41" s="1" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="O41" s="1"/>
       <c r="P41" s="1"/>
       <c r="Q41" s="1"/>
       <c r="R41" s="1" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
     </row>
     <row r="42" spans="1:18" x14ac:dyDescent="0.3">
@@ -5827,43 +5827,43 @@
         <v>41</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C42" s="1" t="s">
         <v>25</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="E42" s="1" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="F42" s="1"/>
       <c r="G42" s="1" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="H42" s="1"/>
       <c r="I42" s="1" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="J42" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="K42" s="1" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="L42" s="1"/>
       <c r="M42" s="1"/>
       <c r="N42" s="1" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="O42" s="4" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="P42" s="1"/>
       <c r="Q42" s="1"/>
       <c r="R42" s="1" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="43" spans="1:18" x14ac:dyDescent="0.3">
@@ -5871,39 +5871,39 @@
         <v>42</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C43" s="1" t="s">
         <v>24</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="E43" s="1" t="s">
         <v>8</v>
       </c>
       <c r="F43" s="1" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="G43" s="1" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="H43" s="1"/>
       <c r="I43" s="1" t="s">
         <v>16</v>
       </c>
       <c r="J43" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="K43" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="L43" s="1" t="s">
         <v>149</v>
-      </c>
-      <c r="L43" s="1" t="s">
-        <v>150</v>
       </c>
       <c r="M43" s="1"/>
       <c r="N43" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="O43" s="1"/>
       <c r="P43" s="1"/>
@@ -5915,45 +5915,45 @@
         <v>43</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C44" s="1" t="s">
         <v>25</v>
       </c>
       <c r="D44" s="1" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="E44" s="1" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="F44" s="1"/>
       <c r="G44" s="1" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="H44" s="1"/>
       <c r="I44" s="1" t="s">
         <v>16</v>
       </c>
       <c r="J44" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="K44" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="L44" s="1" t="s">
         <v>154</v>
       </c>
-      <c r="L44" s="1" t="s">
+      <c r="M44" s="1" t="s">
         <v>155</v>
       </c>
-      <c r="M44" s="1" t="s">
+      <c r="N44" s="1" t="s">
         <v>156</v>
-      </c>
-      <c r="N44" s="1" t="s">
-        <v>157</v>
       </c>
       <c r="O44" s="1"/>
       <c r="P44" s="1"/>
       <c r="Q44" s="1"/>
       <c r="R44" s="1" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="45" spans="1:18" x14ac:dyDescent="0.3">
@@ -5967,7 +5967,7 @@
         <v>24</v>
       </c>
       <c r="D45" s="1" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="E45" s="1" t="s">
         <v>11</v>
@@ -5985,7 +5985,7 @@
         <v>16</v>
       </c>
       <c r="J45" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="K45" s="6" t="s">
         <v>62</v>
@@ -6013,51 +6013,51 @@
         <v>45</v>
       </c>
       <c r="B46" s="7" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="C46" s="7" t="s">
         <v>24</v>
       </c>
       <c r="D46" s="7" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="E46" s="7" t="s">
+        <v>289</v>
+      </c>
+      <c r="F46" s="1" t="s">
         <v>290</v>
-      </c>
-      <c r="F46" s="1" t="s">
-        <v>291</v>
       </c>
       <c r="G46" s="1"/>
       <c r="H46" s="7" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="I46" s="1" t="s">
         <v>16</v>
       </c>
       <c r="J46" s="7" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="K46" s="7" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="L46" s="1"/>
       <c r="M46" s="1" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="N46" s="7" t="s">
         <v>17</v>
       </c>
       <c r="O46" s="1"/>
       <c r="P46" s="1" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="Q46" s="1"/>
       <c r="R46" s="1" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:R45" xr:uid="{00000000-0009-0000-0000-000001000000}"/>
+  <autoFilter ref="A1:R46" xr:uid="{00000000-0009-0000-0000-000001000000}"/>
   <hyperlinks>
     <hyperlink ref="R45" r:id="rId1" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
   </hyperlinks>
@@ -6071,7 +6071,7 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C30" sqref="C30"/>
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Lotus Pond details updated
</commit_message>
<xml_diff>
--- a/ASRProps-Final.xlsx
+++ b/ASRProps-Final.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24026"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/a063b81c7d42b926/Documents/ASR-Props/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="11" documentId="11_B65B585BC469815E41FBBAE2ED8C4BDFAD7A2CD5" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{636F438D-66CD-4D50-845E-A1450F337620}"/>
+  <xr:revisionPtr revIDLastSave="146" documentId="11_B65B585BC469815E41FBBAE2ED8C4BDFAD7A2CD5" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1F6D7C2D-032D-4F33-8232-C6407AF46559}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Property Details'!$A$1:$R$46</definedName>
   </definedNames>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="191029"/>
   <pivotCaches>
     <pivotCache cacheId="0" r:id="rId4"/>
   </pivotCaches>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="641" uniqueCount="292">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="708" uniqueCount="323">
   <si>
     <t>S No</t>
   </si>
@@ -916,12 +916,109 @@
   </si>
   <si>
     <t>Plot No 273</t>
+  </si>
+  <si>
+    <t>1500 Sq Yards</t>
+  </si>
+  <si>
+    <t>Sanjay Jain Kondapur</t>
+  </si>
+  <si>
+    <t>Kondapur</t>
+  </si>
+  <si>
+    <t>Raghavendra Colony</t>
+  </si>
+  <si>
+    <t>Plot No 29-B</t>
+  </si>
+  <si>
+    <t>250 Sq Yards</t>
+  </si>
+  <si>
+    <t>3.50Cr</t>
+  </si>
+  <si>
+    <t>https://www.google.com/maps/place/17%C2%B028'10.3%22N+78%C2%B021'48.5%22E/@17.4695125,78.3632022,20z/data=!4m5!3m4!1s0x0:0x0!8m2!3d17.4695125!4d78.3634758?hl=en</t>
+  </si>
+  <si>
+    <t>Sultan Agent</t>
+  </si>
+  <si>
+    <t>Raod No 44</t>
+  </si>
+  <si>
+    <t>Plot no 853</t>
+  </si>
+  <si>
+    <t>1346 Sq Yards</t>
+  </si>
+  <si>
+    <t>2.80L</t>
+  </si>
+  <si>
+    <t>Cheque Payment</t>
+  </si>
+  <si>
+    <t>SHE by Sai Priya</t>
+  </si>
+  <si>
+    <t>https://www.google.com/maps/place/17%C2%B025'52.6%22N+78%C2%B024'09.7%22E/@17.4312732,78.4005156,17z/data=!3m1!4b1!4m5!3m4!1s0x0:0x0!8m2!3d17.4312732!4d78.4027043?hl=en</t>
+  </si>
+  <si>
+    <t>Road No 44A</t>
+  </si>
+  <si>
+    <t>1391 Sq Yards</t>
+  </si>
+  <si>
+    <t>Plot No 839N</t>
+  </si>
+  <si>
+    <t>Hero Prabas Home Lane</t>
+  </si>
+  <si>
+    <t>https://www.google.com/maps/place/17%C2%B025'54.9%22N+78%C2%B024'11.4%22E/@17.4319041,78.4009844,17z/data=!3m1!4b1!4m5!3m4!1s0x0:0x0!8m2!3d17.4319041!4d78.4031731?hl=en======================</t>
+  </si>
+  <si>
+    <t>Beside CM Jagan House</t>
+  </si>
+  <si>
+    <t>Road No 12, Lotus Pond</t>
+  </si>
+  <si>
+    <t>2873 Sq Yards</t>
+  </si>
+  <si>
+    <t>NORTH SOUTH</t>
+  </si>
+  <si>
+    <t>https://www.google.com/maps/place/17%C2%B024'45.1%22N+78%C2%B025'15.1%22E/@17.412531,78.4186593,17z/data=!3m1!4b1!4m6!3m5!1s0!7e2!8m2!3d17.412531!4d78.4208484</t>
+  </si>
+  <si>
+    <t>Sq Yards</t>
+  </si>
+  <si>
+    <t>GVK Side</t>
+  </si>
+  <si>
+    <t>Rajesh Side</t>
+  </si>
+  <si>
+    <t>Total Price</t>
+  </si>
+  <si>
+    <t>Total</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="2">
+    <numFmt numFmtId="164" formatCode="&quot;₹&quot;\ #,##0.00"/>
+    <numFmt numFmtId="165" formatCode="&quot;₹&quot;\ #,##0.00;[Red]&quot;₹&quot;\ #,##0.00"/>
+  </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -987,7 +1084,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1025,6 +1122,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="165" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2950,7 +3052,7 @@
   <dimension ref="A3:E72"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3890,10 +3992,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:R46"/>
+  <dimension ref="A1:R51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="G46" sqref="G46"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="B52" sqref="B52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="15.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6056,8 +6158,233 @@
         <v>288</v>
       </c>
     </row>
+    <row r="47" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A47" s="16">
+        <v>46</v>
+      </c>
+      <c r="B47" s="7" t="s">
+        <v>114</v>
+      </c>
+      <c r="C47" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="D47" s="7" t="s">
+        <v>273</v>
+      </c>
+      <c r="E47" s="7" t="s">
+        <v>85</v>
+      </c>
+      <c r="F47" s="1"/>
+      <c r="G47" s="1"/>
+      <c r="H47" s="1"/>
+      <c r="I47" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="J47" s="7" t="s">
+        <v>89</v>
+      </c>
+      <c r="K47" s="7" t="s">
+        <v>292</v>
+      </c>
+      <c r="L47" s="1"/>
+      <c r="M47" s="1"/>
+      <c r="N47" s="1"/>
+      <c r="O47" s="1"/>
+      <c r="P47" s="1"/>
+      <c r="Q47" s="1"/>
+      <c r="R47" s="1"/>
+    </row>
+    <row r="48" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A48" s="16">
+        <v>47</v>
+      </c>
+      <c r="B48" s="7" t="s">
+        <v>293</v>
+      </c>
+      <c r="C48" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="D48" s="7" t="s">
+        <v>276</v>
+      </c>
+      <c r="E48" s="7" t="s">
+        <v>294</v>
+      </c>
+      <c r="F48" s="7" t="s">
+        <v>295</v>
+      </c>
+      <c r="G48" s="1"/>
+      <c r="H48" s="7" t="s">
+        <v>296</v>
+      </c>
+      <c r="I48" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="J48" s="7" t="s">
+        <v>89</v>
+      </c>
+      <c r="K48" s="7" t="s">
+        <v>297</v>
+      </c>
+      <c r="L48" s="1"/>
+      <c r="M48" s="1"/>
+      <c r="N48" s="1" t="s">
+        <v>298</v>
+      </c>
+      <c r="O48" s="1"/>
+      <c r="P48" s="1"/>
+      <c r="Q48" s="1"/>
+      <c r="R48" s="1" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="49" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A49" s="16">
+        <v>48</v>
+      </c>
+      <c r="B49" s="7" t="s">
+        <v>300</v>
+      </c>
+      <c r="C49" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="D49" s="7" t="s">
+        <v>273</v>
+      </c>
+      <c r="E49" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="F49" s="1"/>
+      <c r="G49" s="1" t="s">
+        <v>301</v>
+      </c>
+      <c r="H49" s="1" t="s">
+        <v>302</v>
+      </c>
+      <c r="I49" s="7" t="s">
+        <v>252</v>
+      </c>
+      <c r="J49" s="7" t="s">
+        <v>89</v>
+      </c>
+      <c r="K49" s="1" t="s">
+        <v>303</v>
+      </c>
+      <c r="L49" s="1"/>
+      <c r="M49" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="N49" s="1" t="s">
+        <v>304</v>
+      </c>
+      <c r="O49" s="1" t="s">
+        <v>305</v>
+      </c>
+      <c r="P49" s="1" t="s">
+        <v>306</v>
+      </c>
+      <c r="Q49" s="1"/>
+      <c r="R49" s="1" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="50" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A50" s="16">
+        <v>49</v>
+      </c>
+      <c r="B50" s="7" t="s">
+        <v>300</v>
+      </c>
+      <c r="C50" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="D50" s="7" t="s">
+        <v>273</v>
+      </c>
+      <c r="E50" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="F50" s="1"/>
+      <c r="G50" s="1" t="s">
+        <v>308</v>
+      </c>
+      <c r="H50" s="1" t="s">
+        <v>310</v>
+      </c>
+      <c r="I50" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="J50" s="7" t="s">
+        <v>89</v>
+      </c>
+      <c r="K50" s="1" t="s">
+        <v>309</v>
+      </c>
+      <c r="L50" s="1"/>
+      <c r="M50" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="N50" s="1" t="s">
+        <v>304</v>
+      </c>
+      <c r="O50" s="1" t="s">
+        <v>305</v>
+      </c>
+      <c r="P50" s="1" t="s">
+        <v>311</v>
+      </c>
+      <c r="Q50" s="1"/>
+      <c r="R50" s="1" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="51" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A51" s="16">
+        <v>50</v>
+      </c>
+      <c r="B51" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="C51" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="D51" s="7" t="s">
+        <v>279</v>
+      </c>
+      <c r="E51" s="7" t="s">
+        <v>185</v>
+      </c>
+      <c r="F51" s="7" t="s">
+        <v>313</v>
+      </c>
+      <c r="G51" s="7" t="s">
+        <v>314</v>
+      </c>
+      <c r="H51" s="1"/>
+      <c r="I51" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="J51" s="7" t="s">
+        <v>89</v>
+      </c>
+      <c r="K51" s="7" t="s">
+        <v>315</v>
+      </c>
+      <c r="L51" s="1"/>
+      <c r="M51" s="7" t="s">
+        <v>316</v>
+      </c>
+      <c r="N51" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="O51" s="1"/>
+      <c r="P51" s="1"/>
+      <c r="Q51" s="1"/>
+      <c r="R51" s="1" t="s">
+        <v>317</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:R46" xr:uid="{00000000-0009-0000-0000-000001000000}"/>
   <hyperlinks>
     <hyperlink ref="R45" r:id="rId1" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
   </hyperlinks>
@@ -6068,14 +6395,142 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+      <selection activeCell="J15" sqref="J15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="10.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.44140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1" s="1"/>
+      <c r="B1" s="1"/>
+      <c r="C1" s="2" t="s">
+        <v>318</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2" s="1"/>
+      <c r="B2" s="1"/>
+      <c r="C2" s="1">
+        <v>1447</v>
+      </c>
+      <c r="D2" s="1">
+        <v>280000</v>
+      </c>
+      <c r="E2" s="17">
+        <f>C2*D2</f>
+        <v>405160000</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
+        <v>319</v>
+      </c>
+      <c r="B3" s="18">
+        <v>7.4999999999999997E-3</v>
+      </c>
+      <c r="C3" s="1"/>
+      <c r="D3" s="1"/>
+      <c r="E3" s="17">
+        <f>B3*E2</f>
+        <v>3038700</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
+        <v>320</v>
+      </c>
+      <c r="B4" s="18">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="C4" s="1"/>
+      <c r="D4" s="1"/>
+      <c r="E4" s="17">
+        <f>B4*E2</f>
+        <v>2025800</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A5" s="1"/>
+      <c r="B5" s="1"/>
+      <c r="C5" s="1"/>
+      <c r="D5" s="2" t="s">
+        <v>322</v>
+      </c>
+      <c r="E5" s="20">
+        <f>SUM(E3:E4)</f>
+        <v>5064500</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A7" s="1"/>
+      <c r="B7" s="1"/>
+      <c r="C7" s="1"/>
+      <c r="D7" s="1">
+        <v>285000</v>
+      </c>
+      <c r="E7" s="19">
+        <f>D7*C2</f>
+        <v>412395000</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A8" s="1" t="s">
+        <v>319</v>
+      </c>
+      <c r="B8" s="18">
+        <v>7.4999999999999997E-3</v>
+      </c>
+      <c r="C8" s="1"/>
+      <c r="D8" s="1"/>
+      <c r="E8" s="19">
+        <f>B8*E7</f>
+        <v>3092962.5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A9" s="1" t="s">
+        <v>320</v>
+      </c>
+      <c r="B9" s="18">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="C9" s="1"/>
+      <c r="D9" s="1"/>
+      <c r="E9" s="19">
+        <f>B9*E7</f>
+        <v>2061975</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A10" s="1"/>
+      <c r="B10" s="1"/>
+      <c r="C10" s="1"/>
+      <c r="D10" s="2" t="s">
+        <v>322</v>
+      </c>
+      <c r="E10" s="21">
+        <f>SUM(E8:E9)</f>
+        <v>5154937.5</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Msg Format is updated
</commit_message>
<xml_diff>
--- a/ASRProps-Final.xlsx
+++ b/ASRProps-Final.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/a063b81c7d42b926/Documents/ASR-Props/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="146" documentId="11_B65B585BC469815E41FBBAE2ED8C4BDFAD7A2CD5" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1F6D7C2D-032D-4F33-8232-C6407AF46559}"/>
+  <xr:revisionPtr revIDLastSave="148" documentId="11_B65B585BC469815E41FBBAE2ED8C4BDFAD7A2CD5" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F96F4258-3557-4AEA-A5BF-E06B5E347873}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -18,7 +18,7 @@
     <sheet name="Home" sheetId="4" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Property Details'!$A$1:$R$46</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Property Details'!$A$1:$R$51</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <pivotCaches>
@@ -4001,6 +4001,7 @@
   <sheetFormatPr defaultColWidth="15.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="4.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12.109375" customWidth="1"/>
     <col min="4" max="4" width="18.6640625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="19.88671875" bestFit="1" customWidth="1"/>
@@ -4518,7 +4519,7 @@
         <v>139</v>
       </c>
       <c r="I11" s="1" t="s">
-        <v>16</v>
+        <v>252</v>
       </c>
       <c r="J11" s="1" t="s">
         <v>89</v>

</xml_diff>